<commit_message>
added new units in hospital
</commit_message>
<xml_diff>
--- a/lsh_data_processing/lsh_coding.xlsx
+++ b/lsh_data_processing/lsh_coding.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rjs/Documents/GitHub/BCS/lsh_data_processing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEBF46A6-F601-6344-B119-80DE16905802}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52AE3751-400A-DB41-AB0F-D73C2FD05C13}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-2460" yWindow="-21140" windowWidth="19780" windowHeight="21140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="76">
   <si>
     <t>text_out_category_raw</t>
   </si>
@@ -205,13 +205,52 @@
     <t>unit_category_all</t>
   </si>
   <si>
-    <t>unit_category_order_all</t>
-  </si>
-  <si>
     <t>Öldrunarlækningadeild F (Lk-L3)</t>
   </si>
   <si>
     <t>inpatient_ward_geriatric</t>
+  </si>
+  <si>
+    <t>Fæðingarvakt (Hb-23B)</t>
+  </si>
+  <si>
+    <t>Fv-A3 RD Speglun H</t>
+  </si>
+  <si>
+    <t>Hb-10E GD Kviðarhols- og brjóstaskurðlækninga</t>
+  </si>
+  <si>
+    <t>Meðgöngu- og sængurlegudeild (Hb-22A)</t>
+  </si>
+  <si>
+    <t>Sk-N2 GD MAN Starfsumhverfisdeild</t>
+  </si>
+  <si>
+    <t>Skurðdeild</t>
+  </si>
+  <si>
+    <t>Speglun</t>
+  </si>
+  <si>
+    <t>Fæðingardeild</t>
+  </si>
+  <si>
+    <t>inpatient_ward_maternity</t>
+  </si>
+  <si>
+    <t>maternity_clinic</t>
+  </si>
+  <si>
+    <t>Göngudeild starfsmanna</t>
+  </si>
+  <si>
+    <t>outpatient_clinic_staff</t>
+  </si>
+  <si>
+    <t>endoscopy_clinic</t>
+  </si>
+  <si>
+    <t>excluded</t>
   </si>
 </sst>
 </file>
@@ -740,20 +779,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" customWidth="1"/>
+    <col min="1" max="1" width="36.5" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
-    <col min="3" max="4" width="18" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -764,16 +804,13 @@
         <v>59</v>
       </c>
       <c r="D1" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="E1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -783,17 +820,14 @@
       <c r="C2" t="s">
         <v>33</v>
       </c>
-      <c r="D2">
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -803,17 +837,14 @@
       <c r="C3" t="s">
         <v>34</v>
       </c>
-      <c r="D3">
-        <v>3</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="D3" t="s">
         <v>34</v>
       </c>
-      <c r="F3">
+      <c r="E3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -823,17 +854,14 @@
       <c r="C4" t="s">
         <v>33</v>
       </c>
-      <c r="D4">
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4">
         <v>1</v>
       </c>
-      <c r="E4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -843,17 +871,14 @@
       <c r="C5" t="s">
         <v>35</v>
       </c>
-      <c r="D5">
-        <v>2</v>
-      </c>
-      <c r="E5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5">
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -863,17 +888,14 @@
       <c r="C6" t="s">
         <v>34</v>
       </c>
-      <c r="D6">
-        <v>3</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="D6" t="s">
         <v>34</v>
       </c>
-      <c r="F6">
+      <c r="E6">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -883,17 +905,14 @@
       <c r="C7" t="s">
         <v>36</v>
       </c>
-      <c r="D7">
-        <v>4</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="D7" t="s">
         <v>36</v>
       </c>
-      <c r="F7">
+      <c r="E7">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -903,17 +922,14 @@
       <c r="C8" t="s">
         <v>35</v>
       </c>
-      <c r="D8">
-        <v>2</v>
-      </c>
-      <c r="E8" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8">
+      <c r="D8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -923,17 +939,14 @@
       <c r="C9" t="s">
         <v>33</v>
       </c>
-      <c r="D9">
+      <c r="D9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9">
         <v>1</v>
       </c>
-      <c r="E9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -943,17 +956,14 @@
       <c r="C10" t="s">
         <v>33</v>
       </c>
-      <c r="D10">
+      <c r="D10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10">
         <v>1</v>
       </c>
-      <c r="E10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -961,36 +971,132 @@
         <v>30</v>
       </c>
       <c r="C11" t="s">
-        <v>62</v>
-      </c>
-      <c r="D11">
-        <v>3</v>
-      </c>
-      <c r="E11" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" t="s">
         <v>34</v>
       </c>
-      <c r="F11">
+      <c r="E11">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B12" t="s">
         <v>30</v>
       </c>
       <c r="C12" t="s">
+        <v>61</v>
+      </c>
+      <c r="D12" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>62</v>
       </c>
-      <c r="D12">
-        <v>3</v>
-      </c>
-      <c r="E12" t="s">
+      <c r="B13" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" t="s">
+        <v>71</v>
+      </c>
+      <c r="D13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" t="s">
+        <v>68</v>
+      </c>
+      <c r="C14" t="s">
+        <v>74</v>
+      </c>
+      <c r="D14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B15" t="s">
+        <v>67</v>
+      </c>
+      <c r="C15" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" t="s">
+        <v>70</v>
+      </c>
+      <c r="D17" t="s">
         <v>34</v>
       </c>
-      <c r="F12">
+      <c r="E17">
         <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B18" t="s">
+        <v>72</v>
+      </c>
+      <c r="C18" t="s">
+        <v>73</v>
+      </c>
+      <c r="D18" t="s">
+        <v>75</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added names of sheets
</commit_message>
<xml_diff>
--- a/lsh_data_processing/lsh_coding.xlsx
+++ b/lsh_data_processing/lsh_coding.xlsx
@@ -8,22 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rjs/Documents/GitHub/BCS/lsh_data_processing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC69B5FA-CD9D-334E-9F14-BEDAB9AEAF1D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{562C797F-F1DB-7F42-BADD-161D56358ADA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-21140" windowWidth="19780" windowHeight="21140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="-21140" windowWidth="19780" windowHeight="21140" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="lsh_covid_groups" sheetId="3" r:id="rId1"/>
     <sheet name="lsh_services" sheetId="4" r:id="rId2"/>
     <sheet name="lsh_unit_categories" sheetId="1" r:id="rId3"/>
     <sheet name="lsh_text_out_categories" sheetId="2" r:id="rId4"/>
+    <sheet name="lsh_sheet_names" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="86">
   <si>
     <t>text_out_category_raw</t>
   </si>
@@ -248,6 +249,39 @@
   </si>
   <si>
     <t>endoscopy_clinic</t>
+  </si>
+  <si>
+    <t>Einangrun - af skjáborði Heilsu</t>
+  </si>
+  <si>
+    <t>Lokaviðtal-Spurning úr forms</t>
+  </si>
+  <si>
+    <t>Einstaklingar</t>
+  </si>
+  <si>
+    <t>Komur og innlagnir</t>
+  </si>
+  <si>
+    <t>Áhættuflokkur ofl úr hóp</t>
+  </si>
+  <si>
+    <t>Fyrsta viðtal úr forms</t>
+  </si>
+  <si>
+    <t>Spurningar úr forms Pivot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NEWS score </t>
+  </si>
+  <si>
+    <t>EG_Skoða gagnagöt</t>
+  </si>
+  <si>
+    <t>Eldra_Spurningar úr forms</t>
+  </si>
+  <si>
+    <t>sheet_name_raw</t>
   </si>
 </sst>
 </file>
@@ -778,7 +812,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
@@ -1228,4 +1262,77 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50D32CD1-884D-D640-99E8-CDE941A3B434}">
+  <dimension ref="A1:A11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="24.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fixing tests and adding path to new data. Also fixed coding excel file
</commit_message>
<xml_diff>
--- a/lsh_data_processing/lsh_coding.xlsx
+++ b/lsh_data_processing/lsh_coding.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10307"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rjs/Documents/GitHub/BCS/lsh_data_processing/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29B2BF62-7635-844C-A035-5CCD5F6381ED}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="27729"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-320" yWindow="-17920" windowWidth="19780" windowHeight="15340" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-32380" yWindow="460" windowWidth="25040" windowHeight="14000" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="lsh_covid_groups" sheetId="3" r:id="rId1"/>
@@ -19,7 +13,12 @@
     <sheet name="lsh_text_out_categories" sheetId="2" r:id="rId4"/>
     <sheet name="lsh_sheet_names" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -290,13 +289,13 @@
     <t>Hb-22B GD Mæðravernd</t>
   </si>
   <si>
-    <t>NEWS score</t>
+    <t xml:space="preserve">NEWS score </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -427,7 +426,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -479,7 +478,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -673,28 +672,28 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7678E24-D474-7A43-9E65-B8032B1FD84B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="29.1640625" customWidth="1"/>
     <col min="2" max="2" width="19.83203125" customWidth="1"/>
     <col min="3" max="3" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>37</v>
       </c>
@@ -705,7 +704,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
         <v>40</v>
       </c>
@@ -716,7 +715,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
         <v>41</v>
       </c>
@@ -727,7 +726,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
         <v>42</v>
       </c>
@@ -738,7 +737,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
         <v>43</v>
       </c>
@@ -749,7 +748,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
         <v>44</v>
       </c>
@@ -762,25 +761,30 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36AB6D07-ADE6-1545-9003-92490C67806D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
+    <sheetView zoomScale="210" zoomScaleNormal="210" zoomScalePageLayoutView="210" workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="15.1640625" customWidth="1"/>
     <col min="2" max="2" width="16.1640625" customWidth="1"/>
     <col min="3" max="3" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>51</v>
       </c>
@@ -791,7 +795,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>54</v>
       </c>
@@ -802,7 +806,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>55</v>
       </c>
@@ -815,18 +819,23 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="36.5" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
@@ -834,7 +843,7 @@
     <col min="4" max="4" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -851,7 +860,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -868,7 +877,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -885,7 +894,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -902,7 +911,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -919,7 +928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -936,7 +945,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -953,7 +962,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -970,7 +979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -987,7 +996,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -1004,7 +1013,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -1021,7 +1030,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5">
       <c r="A12" s="2" t="s">
         <v>60</v>
       </c>
@@ -1038,7 +1047,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>62</v>
       </c>
@@ -1055,7 +1064,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>63</v>
       </c>
@@ -1072,7 +1081,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5">
       <c r="A15" s="2" t="s">
         <v>64</v>
       </c>
@@ -1089,7 +1098,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5">
       <c r="A16" s="2" t="s">
         <v>65</v>
       </c>
@@ -1106,7 +1115,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5">
       <c r="A17" s="2" t="s">
         <v>66</v>
       </c>
@@ -1123,7 +1132,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5">
       <c r="A18" s="1" t="s">
         <v>85</v>
       </c>
@@ -1140,7 +1149,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>86</v>
       </c>
@@ -1157,7 +1166,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5">
       <c r="A20" s="1" t="s">
         <v>87</v>
       </c>
@@ -1176,25 +1185,30 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D4F8184-5026-8E41-99B1-0CDE69C1468B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="31" customWidth="1"/>
     <col min="2" max="2" width="25.1640625" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1208,7 +1222,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1222,7 +1236,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1236,7 +1250,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1250,7 +1264,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1264,7 +1278,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1278,7 +1292,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1292,7 +1306,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -1306,7 +1320,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -1322,78 +1336,88 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50D32CD1-884D-D640-99E8-CDE941A3B434}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="24.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1">
       <c r="A3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1">
       <c r="A4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1">
       <c r="A5" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1">
       <c r="A6" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:1">
       <c r="A7" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:1">
       <c r="A8" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:1">
       <c r="A9" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:1">
       <c r="A10" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:1">
       <c r="A11" t="s">
         <v>83</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
change sheet name because of addition to coding excel file
</commit_message>
<xml_diff>
--- a/lsh_data_processing/lsh_coding.xlsx
+++ b/lsh_data_processing/lsh_coding.xlsx
@@ -4,14 +4,15 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="27729"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-32380" yWindow="460" windowWidth="25040" windowHeight="14000" activeTab="4"/>
+    <workbookView xWindow="-32380" yWindow="460" windowWidth="25040" windowHeight="14000" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="lsh_covid_groups" sheetId="3" r:id="rId1"/>
     <sheet name="lsh_services" sheetId="4" r:id="rId2"/>
     <sheet name="lsh_unit_categories" sheetId="1" r:id="rId3"/>
     <sheet name="lsh_text_out_categories" sheetId="2" r:id="rId4"/>
-    <sheet name="lsh_sheet_names" sheetId="5" r:id="rId5"/>
+    <sheet name="clinical_assessment_categories" sheetId="6" r:id="rId5"/>
+    <sheet name="lsh_sheet_names" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="107">
   <si>
     <t>text_out_category_raw</t>
   </si>
@@ -290,13 +291,67 @@
   </si>
   <si>
     <t xml:space="preserve">NEWS score </t>
+  </si>
+  <si>
+    <t>clinical_assessment_category_raw</t>
+  </si>
+  <si>
+    <t>clinical_assessment_category_all</t>
+  </si>
+  <si>
+    <t>clinical_assessment_category_simple</t>
+  </si>
+  <si>
+    <t>Blár</t>
+  </si>
+  <si>
+    <t>Brúnn</t>
+  </si>
+  <si>
+    <t>Grænn</t>
+  </si>
+  <si>
+    <t>Hvítur</t>
+  </si>
+  <si>
+    <t>Óskilgreint</t>
+  </si>
+  <si>
+    <t>Rauður</t>
+  </si>
+  <si>
+    <t>blue</t>
+  </si>
+  <si>
+    <t>brown</t>
+  </si>
+  <si>
+    <t>green</t>
+  </si>
+  <si>
+    <t>white</t>
+  </si>
+  <si>
+    <t>unknown</t>
+  </si>
+  <si>
+    <t>red</t>
+  </si>
+  <si>
+    <t>Gulur</t>
+  </si>
+  <si>
+    <t>yellow</t>
+  </si>
+  <si>
+    <t>clinical_assessment_order_simple</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -315,6 +370,29 @@
       <color rgb="FF333333"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -355,10 +433,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -366,8 +456,21 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="13">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -672,7 +775,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -832,7 +935,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -840,7 +943,8 @@
     <col min="1" max="1" width="36.5" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
     <col min="3" max="3" width="21.1640625" customWidth="1"/>
-    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="4" max="4" width="29.83203125" customWidth="1"/>
+    <col min="5" max="5" width="25.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1346,9 +1450,148 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="28.33203125" customWidth="1"/>
+    <col min="2" max="2" width="30.83203125" customWidth="1"/>
+    <col min="3" max="3" width="32.33203125" customWidth="1"/>
+    <col min="4" max="4" width="33" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C5" t="s">
+        <v>103</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B6" t="s">
+        <v>101</v>
+      </c>
+      <c r="C6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>96</v>
+      </c>
+      <c r="B7" t="s">
+        <v>102</v>
+      </c>
+      <c r="C7" t="s">
+        <v>102</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>97</v>
+      </c>
+      <c r="B8" t="s">
+        <v>103</v>
+      </c>
+      <c r="C8" t="s">
+        <v>103</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added categories and sheet for ventilators
</commit_message>
<xml_diff>
--- a/lsh_data_processing/lsh_coding.xlsx
+++ b/lsh_data_processing/lsh_coding.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="27729"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10307"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rjs/projects/covid/BCS/lsh_data_processing/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AFFE3E6-5276-9B46-8046-824D978FBF25}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32380" yWindow="460" windowWidth="25040" windowHeight="14000" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25040" windowHeight="14000" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="lsh_covid_groups" sheetId="3" r:id="rId1"/>
@@ -14,7 +20,7 @@
     <sheet name="clinical_assessment_categories" sheetId="6" r:id="rId5"/>
     <sheet name="lsh_sheet_names" sheetId="5" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="111">
   <si>
     <t>text_out_category_raw</t>
   </si>
@@ -345,12 +351,24 @@
   </si>
   <si>
     <t>clinical_assessment_order_simple</t>
+  </si>
+  <si>
+    <t>Öndunarvélar - tímar</t>
+  </si>
+  <si>
+    <t>Fv-B3 GD Æðaskurðlækninga</t>
+  </si>
+  <si>
+    <t>Sjúkrahótel Landspítala (Ám9)</t>
+  </si>
+  <si>
+    <t>patient_hotel</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -775,28 +793,28 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="29.1640625" customWidth="1"/>
     <col min="2" max="2" width="19.83203125" customWidth="1"/>
     <col min="3" max="3" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>37</v>
       </c>
@@ -807,7 +825,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>40</v>
       </c>
@@ -818,7 +836,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>41</v>
       </c>
@@ -829,7 +847,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>42</v>
       </c>
@@ -840,7 +858,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>43</v>
       </c>
@@ -851,7 +869,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>44</v>
       </c>
@@ -873,21 +891,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView zoomScale="210" zoomScaleNormal="210" zoomScalePageLayoutView="210" workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.1640625" customWidth="1"/>
     <col min="2" max="2" width="16.1640625" customWidth="1"/>
     <col min="3" max="3" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>51</v>
       </c>
@@ -898,7 +916,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>54</v>
       </c>
@@ -909,7 +927,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>55</v>
       </c>
@@ -931,14 +949,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="36.5" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
@@ -947,7 +965,7 @@
     <col min="5" max="5" width="25.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -964,7 +982,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -981,7 +999,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -998,7 +1016,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -1015,7 +1033,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -1032,7 +1050,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -1049,7 +1067,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -1066,7 +1084,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -1083,7 +1101,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -1100,7 +1118,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -1117,7 +1135,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -1134,7 +1152,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>60</v>
       </c>
@@ -1151,7 +1169,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>62</v>
       </c>
@@ -1168,7 +1186,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>63</v>
       </c>
@@ -1185,7 +1203,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>64</v>
       </c>
@@ -1202,7 +1220,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>65</v>
       </c>
@@ -1219,7 +1237,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>66</v>
       </c>
@@ -1236,7 +1254,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>85</v>
       </c>
@@ -1253,7 +1271,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>86</v>
       </c>
@@ -1270,7 +1288,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>87</v>
       </c>
@@ -1284,6 +1302,40 @@
         <v>10</v>
       </c>
       <c r="E20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>108</v>
+      </c>
+      <c r="B21" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>109</v>
+      </c>
+      <c r="B22" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" t="s">
+        <v>110</v>
+      </c>
+      <c r="D22" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22">
         <v>1</v>
       </c>
     </row>
@@ -1298,21 +1350,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="31" customWidth="1"/>
     <col min="2" max="2" width="25.1640625" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1326,7 +1378,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1340,7 +1392,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1354,7 +1406,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1368,7 +1420,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1382,7 +1434,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1396,7 +1448,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1410,7 +1462,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -1424,7 +1476,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -1449,14 +1501,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="28.33203125" customWidth="1"/>
     <col min="2" max="2" width="30.83203125" customWidth="1"/>
@@ -1464,7 +1516,7 @@
     <col min="4" max="4" width="33" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>89</v>
       </c>
@@ -1478,7 +1530,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>92</v>
       </c>
@@ -1492,7 +1544,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>93</v>
       </c>
@@ -1506,7 +1558,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>94</v>
       </c>
@@ -1520,7 +1572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>104</v>
       </c>
@@ -1534,7 +1586,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>95</v>
       </c>
@@ -1548,7 +1600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>96</v>
       </c>
@@ -1562,7 +1614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>97</v>
       </c>
@@ -1588,71 +1640,76 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding orders for unsimplified categories of clinical assessment
</commit_message>
<xml_diff>
--- a/lsh_data_processing/lsh_coding.xlsx
+++ b/lsh_data_processing/lsh_coding.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="27729"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maestro/projects/covid/BCS/lsh_data_processing/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F672ECD7-EF05-E84B-AFA5-0834ECF70A4A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32380" yWindow="460" windowWidth="25040" windowHeight="14000" firstSheet="2" activeTab="6"/>
+    <workbookView xWindow="28780" yWindow="-1720" windowWidth="38400" windowHeight="21600" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="lsh_covid_groups" sheetId="3" r:id="rId1"/>
@@ -15,7 +21,7 @@
     <sheet name="lsh_sheet_names" sheetId="5" r:id="rId6"/>
     <sheet name="priority_categories" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -25,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="118">
   <si>
     <t>text_out_category_raw</t>
   </si>
@@ -376,12 +382,15 @@
   </si>
   <si>
     <t>priority_category_order_simple</t>
+  </si>
+  <si>
+    <t>clinical_assessment_category_order_all</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -810,28 +819,28 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="29.1640625" customWidth="1"/>
     <col min="2" max="2" width="19.83203125" customWidth="1"/>
     <col min="3" max="3" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>37</v>
       </c>
@@ -842,7 +851,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>40</v>
       </c>
@@ -853,7 +862,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>41</v>
       </c>
@@ -864,7 +873,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>42</v>
       </c>
@@ -875,7 +884,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>43</v>
       </c>
@@ -886,7 +895,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>44</v>
       </c>
@@ -908,21 +917,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView zoomScale="210" zoomScaleNormal="210" zoomScalePageLayoutView="210" workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.1640625" customWidth="1"/>
     <col min="2" max="2" width="16.1640625" customWidth="1"/>
     <col min="3" max="3" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>51</v>
       </c>
@@ -933,7 +942,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>54</v>
       </c>
@@ -944,7 +953,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>55</v>
       </c>
@@ -966,14 +975,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="36.5" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
@@ -982,7 +991,7 @@
     <col min="5" max="5" width="25.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -999,7 +1008,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -1016,7 +1025,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -1033,7 +1042,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -1050,7 +1059,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -1067,7 +1076,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -1084,7 +1093,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -1101,7 +1110,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -1118,7 +1127,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -1135,7 +1144,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -1152,7 +1161,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -1169,7 +1178,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>60</v>
       </c>
@@ -1186,7 +1195,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>62</v>
       </c>
@@ -1203,7 +1212,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>63</v>
       </c>
@@ -1220,7 +1229,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>64</v>
       </c>
@@ -1237,7 +1246,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>65</v>
       </c>
@@ -1254,7 +1263,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>66</v>
       </c>
@@ -1271,7 +1280,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>85</v>
       </c>
@@ -1288,7 +1297,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>86</v>
       </c>
@@ -1305,7 +1314,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>87</v>
       </c>
@@ -1333,21 +1342,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="31" customWidth="1"/>
     <col min="2" max="2" width="25.1640625" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1361,7 +1370,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1375,7 +1384,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1389,7 +1398,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1403,7 +1412,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1417,7 +1426,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1431,7 +1440,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1445,7 +1454,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -1459,7 +1468,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -1484,22 +1493,22 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="28.33203125" customWidth="1"/>
     <col min="2" max="2" width="30.83203125" customWidth="1"/>
     <col min="3" max="3" width="32.33203125" customWidth="1"/>
-    <col min="4" max="4" width="33" customWidth="1"/>
+    <col min="4" max="5" width="33" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>89</v>
       </c>
@@ -1512,8 +1521,11 @@
       <c r="D1" s="3" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>92</v>
       </c>
@@ -1526,8 +1538,11 @@
       <c r="D2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>93</v>
       </c>
@@ -1540,8 +1555,11 @@
       <c r="D3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>94</v>
       </c>
@@ -1554,8 +1572,11 @@
       <c r="D4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="E4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>104</v>
       </c>
@@ -1568,8 +1589,11 @@
       <c r="D5">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="E5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>95</v>
       </c>
@@ -1582,8 +1606,11 @@
       <c r="D6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="E6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>96</v>
       </c>
@@ -1596,8 +1623,11 @@
       <c r="D7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="E7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>97</v>
       </c>
@@ -1609,6 +1639,9 @@
       </c>
       <c r="D8">
         <v>1</v>
+      </c>
+      <c r="E8">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -1623,69 +1656,69 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>83</v>
       </c>
@@ -1701,14 +1734,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="29.83203125" customWidth="1"/>
     <col min="2" max="2" width="27.1640625" customWidth="1"/>
@@ -1716,7 +1749,7 @@
     <col min="4" max="4" width="34.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>113</v>
       </c>
@@ -1730,7 +1763,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>107</v>
       </c>
@@ -1744,7 +1777,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>108</v>
       </c>
@@ -1758,7 +1791,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>109</v>
       </c>

</xml_diff>

<commit_message>
Added comorbidities and n of comorbidities to first_interview and n comorbidities to indivis_extended
</commit_message>
<xml_diff>
--- a/lsh_data_processing/lsh_coding.xlsx
+++ b/lsh_data_processing/lsh_coding.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maestro/projects/covid/BCS/lsh_data_processing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F672ECD7-EF05-E84B-AFA5-0834ECF70A4A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2902553-F4CF-C345-A143-ADD26397D714}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28780" yWindow="-1720" windowWidth="38400" windowHeight="21600" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28440" yWindow="-1720" windowWidth="19200" windowHeight="21600" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="lsh_covid_groups" sheetId="3" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="clinical_assessment_categories" sheetId="6" r:id="rId5"/>
     <sheet name="lsh_sheet_names" sheetId="5" r:id="rId6"/>
     <sheet name="priority_categories" sheetId="7" r:id="rId7"/>
+    <sheet name="comorbidities" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="140001"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="141">
   <si>
     <t>text_out_category_raw</t>
   </si>
@@ -385,6 +386,75 @@
   </si>
   <si>
     <t>clinical_assessment_category_order_all</t>
+  </si>
+  <si>
+    <t>comorbidities_raw</t>
+  </si>
+  <si>
+    <t>Almennt hraust/ur</t>
+  </si>
+  <si>
+    <t>Krabbamein (meðferð lokið/í remission)</t>
+  </si>
+  <si>
+    <t>Krabbamein (í meðferð/virkur sjúkdómur)</t>
+  </si>
+  <si>
+    <t>Háþrýstingur</t>
+  </si>
+  <si>
+    <t>Sykursýki I</t>
+  </si>
+  <si>
+    <t>Sykursýki II</t>
+  </si>
+  <si>
+    <t>Lungasjúkdómur</t>
+  </si>
+  <si>
+    <t>Langvinnur nýrnasjúkdómur</t>
+  </si>
+  <si>
+    <t>comorbidities_names</t>
+  </si>
+  <si>
+    <t>healthy</t>
+  </si>
+  <si>
+    <t>cancer_remission</t>
+  </si>
+  <si>
+    <t>cancer_active</t>
+  </si>
+  <si>
+    <t>cardiovasc</t>
+  </si>
+  <si>
+    <t>hypertension</t>
+  </si>
+  <si>
+    <t>dm1</t>
+  </si>
+  <si>
+    <t>dm2</t>
+  </si>
+  <si>
+    <t>kidney_disease</t>
+  </si>
+  <si>
+    <t>pulmonary_disease</t>
+  </si>
+  <si>
+    <t>inflammatory_disease</t>
+  </si>
+  <si>
+    <t>comorbidities_included</t>
+  </si>
+  <si>
+    <t>Bólgusjúkdómar</t>
+  </si>
+  <si>
+    <t>Hjarta-og æðasjúkdómur</t>
   </si>
 </sst>
 </file>
@@ -1496,7 +1566,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -1813,4 +1883,144 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E595DE6E-CBA1-634A-B045-38D514B9DB87}">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="36" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>140</v>
+      </c>
+      <c r="B5" t="s">
+        <v>131</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>122</v>
+      </c>
+      <c r="B6" t="s">
+        <v>132</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>123</v>
+      </c>
+      <c r="B7" t="s">
+        <v>133</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>124</v>
+      </c>
+      <c r="B8" t="s">
+        <v>134</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>125</v>
+      </c>
+      <c r="B9" t="s">
+        <v>136</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>126</v>
+      </c>
+      <c r="B10" t="s">
+        <v>135</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>139</v>
+      </c>
+      <c r="B11" t="s">
+        <v>137</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added new categories and updated for clinical assessment procerssing
</commit_message>
<xml_diff>
--- a/lsh_data_processing/lsh_coding.xlsx
+++ b/lsh_data_processing/lsh_coding.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rjs/projects/covid/BCS/lsh_data_processing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D20EAD4-702A-9747-A9C8-C414255F0AEE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A57B2FF4-19D2-414A-8005-ED25D94DA78A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1380" yWindow="-18800" windowWidth="25040" windowHeight="14000" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3040" yWindow="-19740" windowWidth="25040" windowHeight="14000" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="lsh_covid_groups" sheetId="3" r:id="rId1"/>
@@ -19,7 +19,8 @@
     <sheet name="lsh_text_out_categories" sheetId="2" r:id="rId4"/>
     <sheet name="clinical_assessment_categories" sheetId="6" r:id="rId5"/>
     <sheet name="lsh_sheet_names" sheetId="5" r:id="rId6"/>
-    <sheet name="Sheet1" sheetId="7" r:id="rId7"/>
+    <sheet name="priority_categories" sheetId="7" r:id="rId7"/>
+    <sheet name="comorbidities" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="140001"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="149">
   <si>
     <t>text_out_category_raw</t>
   </si>
@@ -367,6 +368,117 @@
   </si>
   <si>
     <t>Klíníska matið - today</t>
+  </si>
+  <si>
+    <t>priority_category_raw</t>
+  </si>
+  <si>
+    <t>priority_category_all</t>
+  </si>
+  <si>
+    <t>priority_category_simple</t>
+  </si>
+  <si>
+    <t>priority_category_order_simple</t>
+  </si>
+  <si>
+    <t>Lágur</t>
+  </si>
+  <si>
+    <t>low</t>
+  </si>
+  <si>
+    <t>Meðal</t>
+  </si>
+  <si>
+    <t>medium</t>
+  </si>
+  <si>
+    <t>Hár</t>
+  </si>
+  <si>
+    <t>high</t>
+  </si>
+  <si>
+    <t>comorbidities_raw</t>
+  </si>
+  <si>
+    <t>comorbidities_names</t>
+  </si>
+  <si>
+    <t>comorbidities_included</t>
+  </si>
+  <si>
+    <t>Almennt hraust/ur</t>
+  </si>
+  <si>
+    <t>healthy</t>
+  </si>
+  <si>
+    <t>Krabbamein (meðferð lokið/í remission)</t>
+  </si>
+  <si>
+    <t>cancer_remission</t>
+  </si>
+  <si>
+    <t>Krabbamein (í meðferð/virkur sjúkdómur)</t>
+  </si>
+  <si>
+    <t>cancer_active</t>
+  </si>
+  <si>
+    <t>Hjarta-og æðasjúkdómur</t>
+  </si>
+  <si>
+    <t>cardiovasc</t>
+  </si>
+  <si>
+    <t>Háþrýstingur</t>
+  </si>
+  <si>
+    <t>hypertension</t>
+  </si>
+  <si>
+    <t>Sykursýki I</t>
+  </si>
+  <si>
+    <t>dm1</t>
+  </si>
+  <si>
+    <t>Sykursýki II</t>
+  </si>
+  <si>
+    <t>dm2</t>
+  </si>
+  <si>
+    <t>Lungasjúkdómur</t>
+  </si>
+  <si>
+    <t>pulmonary_disease</t>
+  </si>
+  <si>
+    <t>Langvinnur nýrnasjúkdómur</t>
+  </si>
+  <si>
+    <t>kidney_disease</t>
+  </si>
+  <si>
+    <t>Bólgusjúkdómar</t>
+  </si>
+  <si>
+    <t>inflammatory_disease</t>
+  </si>
+  <si>
+    <t>Fv-G2 BM Göngu</t>
+  </si>
+  <si>
+    <t>Fv-G3 GD Bráðalækninga</t>
+  </si>
+  <si>
+    <t>Fv-B7 DD Gigt- og alm.lyfl.</t>
+  </si>
+  <si>
+    <t>Dagdeild</t>
   </si>
 </sst>
 </file>
@@ -954,10 +1066,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1343,6 +1455,57 @@
         <v>1</v>
       </c>
     </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>145</v>
+      </c>
+      <c r="B23" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" t="s">
+        <v>35</v>
+      </c>
+      <c r="D23" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>146</v>
+      </c>
+      <c r="B24" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>147</v>
+      </c>
+      <c r="B25" t="s">
+        <v>148</v>
+      </c>
+      <c r="C25" t="s">
+        <v>35</v>
+      </c>
+      <c r="D25" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1357,7 +1520,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -1733,14 +1896,212 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8023469F-76F5-624D-BF66-0A486118095E}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C4" t="s">
+        <v>121</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B03F9D6-05FA-864A-B0C5-D8AE08309FFE}">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="30" customWidth="1"/>
+    <col min="2" max="2" width="22.83203125" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>131</v>
+      </c>
+      <c r="B5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>133</v>
+      </c>
+      <c r="B6" t="s">
+        <v>134</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>135</v>
+      </c>
+      <c r="B7" t="s">
+        <v>136</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>137</v>
+      </c>
+      <c r="B8" t="s">
+        <v>138</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>139</v>
+      </c>
+      <c r="B9" t="s">
+        <v>140</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>141</v>
+      </c>
+      <c r="B10" t="s">
+        <v>142</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>143</v>
+      </c>
+      <c r="B11" t="s">
+        <v>144</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
new coding excel file
</commit_message>
<xml_diff>
--- a/lsh_data_processing/lsh_coding.xlsx
+++ b/lsh_data_processing/lsh_coding.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10307"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maestro/projects/covid/BCS/lsh_data_processing/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rjs/projects/covid/BCS/lsh_data_processing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2902553-F4CF-C345-A143-ADD26397D714}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{368F3BB7-1505-2F4F-8D0B-D2138D085D8B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28440" yWindow="-1720" windowWidth="19200" windowHeight="21600" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3040" yWindow="-19740" windowWidth="25040" windowHeight="14000" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="lsh_covid_groups" sheetId="3" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="150">
   <si>
     <t>text_out_category_raw</t>
   </si>
@@ -352,109 +352,136 @@
     <t>yellow</t>
   </si>
   <si>
+    <t>Fv-B3 GD Æðaskurðlækninga</t>
+  </si>
+  <si>
+    <t>Sjúkrahótel Landspítala (Ám9)</t>
+  </si>
+  <si>
+    <t>patient_hotel</t>
+  </si>
+  <si>
+    <t>Öndunarvél - tímar</t>
+  </si>
+  <si>
+    <t>Klíníska matið - today</t>
+  </si>
+  <si>
+    <t>priority_category_raw</t>
+  </si>
+  <si>
+    <t>priority_category_all</t>
+  </si>
+  <si>
+    <t>priority_category_simple</t>
+  </si>
+  <si>
+    <t>priority_category_order_simple</t>
+  </si>
+  <si>
+    <t>Lágur</t>
+  </si>
+  <si>
+    <t>low</t>
+  </si>
+  <si>
+    <t>Meðal</t>
+  </si>
+  <si>
+    <t>medium</t>
+  </si>
+  <si>
+    <t>Hár</t>
+  </si>
+  <si>
+    <t>high</t>
+  </si>
+  <si>
+    <t>comorbidities_raw</t>
+  </si>
+  <si>
+    <t>comorbidities_names</t>
+  </si>
+  <si>
+    <t>comorbidities_included</t>
+  </si>
+  <si>
+    <t>Almennt hraust/ur</t>
+  </si>
+  <si>
+    <t>healthy</t>
+  </si>
+  <si>
+    <t>Krabbamein (meðferð lokið/í remission)</t>
+  </si>
+  <si>
+    <t>cancer_remission</t>
+  </si>
+  <si>
+    <t>Krabbamein (í meðferð/virkur sjúkdómur)</t>
+  </si>
+  <si>
+    <t>cancer_active</t>
+  </si>
+  <si>
+    <t>Hjarta-og æðasjúkdómur</t>
+  </si>
+  <si>
+    <t>cardiovasc</t>
+  </si>
+  <si>
+    <t>Háþrýstingur</t>
+  </si>
+  <si>
+    <t>hypertension</t>
+  </si>
+  <si>
+    <t>Sykursýki I</t>
+  </si>
+  <si>
+    <t>dm1</t>
+  </si>
+  <si>
+    <t>Sykursýki II</t>
+  </si>
+  <si>
+    <t>dm2</t>
+  </si>
+  <si>
+    <t>Lungasjúkdómur</t>
+  </si>
+  <si>
+    <t>pulmonary_disease</t>
+  </si>
+  <si>
+    <t>Langvinnur nýrnasjúkdómur</t>
+  </si>
+  <si>
+    <t>kidney_disease</t>
+  </si>
+  <si>
+    <t>Bólgusjúkdómar</t>
+  </si>
+  <si>
+    <t>inflammatory_disease</t>
+  </si>
+  <si>
+    <t>Fv-G2 BM Göngu</t>
+  </si>
+  <si>
+    <t>Fv-G3 GD Bráðalækninga</t>
+  </si>
+  <si>
+    <t>Fv-B7 DD Gigt- og alm.lyfl.</t>
+  </si>
+  <si>
+    <t>Dagdeild</t>
+  </si>
+  <si>
     <t>clinical_assessment_category_order_simple</t>
   </si>
   <si>
-    <t>Lágur</t>
-  </si>
-  <si>
-    <t>Meðal</t>
-  </si>
-  <si>
-    <t>Hár</t>
-  </si>
-  <si>
-    <t>low</t>
-  </si>
-  <si>
-    <t>medium</t>
-  </si>
-  <si>
-    <t>high</t>
-  </si>
-  <si>
-    <t>priority_category_raw</t>
-  </si>
-  <si>
-    <t>priority_category_all</t>
-  </si>
-  <si>
-    <t>priority_category_simple</t>
-  </si>
-  <si>
-    <t>priority_category_order_simple</t>
-  </si>
-  <si>
     <t>clinical_assessment_category_order_all</t>
-  </si>
-  <si>
-    <t>comorbidities_raw</t>
-  </si>
-  <si>
-    <t>Almennt hraust/ur</t>
-  </si>
-  <si>
-    <t>Krabbamein (meðferð lokið/í remission)</t>
-  </si>
-  <si>
-    <t>Krabbamein (í meðferð/virkur sjúkdómur)</t>
-  </si>
-  <si>
-    <t>Háþrýstingur</t>
-  </si>
-  <si>
-    <t>Sykursýki I</t>
-  </si>
-  <si>
-    <t>Sykursýki II</t>
-  </si>
-  <si>
-    <t>Lungasjúkdómur</t>
-  </si>
-  <si>
-    <t>Langvinnur nýrnasjúkdómur</t>
-  </si>
-  <si>
-    <t>comorbidities_names</t>
-  </si>
-  <si>
-    <t>healthy</t>
-  </si>
-  <si>
-    <t>cancer_remission</t>
-  </si>
-  <si>
-    <t>cancer_active</t>
-  </si>
-  <si>
-    <t>cardiovasc</t>
-  </si>
-  <si>
-    <t>hypertension</t>
-  </si>
-  <si>
-    <t>dm1</t>
-  </si>
-  <si>
-    <t>dm2</t>
-  </si>
-  <si>
-    <t>kidney_disease</t>
-  </si>
-  <si>
-    <t>pulmonary_disease</t>
-  </si>
-  <si>
-    <t>inflammatory_disease</t>
-  </si>
-  <si>
-    <t>comorbidities_included</t>
-  </si>
-  <si>
-    <t>Bólgusjúkdómar</t>
-  </si>
-  <si>
-    <t>Hjarta-og æðasjúkdómur</t>
   </si>
 </sst>
 </file>
@@ -543,10 +570,8 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -570,21 +595,19 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -643,7 +666,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -695,7 +718,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1046,10 +1069,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView topLeftCell="A5" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1398,6 +1421,91 @@
         <v>10</v>
       </c>
       <c r="E20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>106</v>
+      </c>
+      <c r="B21" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>107</v>
+      </c>
+      <c r="B22" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" t="s">
+        <v>108</v>
+      </c>
+      <c r="D22" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>144</v>
+      </c>
+      <c r="B23" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" t="s">
+        <v>35</v>
+      </c>
+      <c r="D23" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>145</v>
+      </c>
+      <c r="B24" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>146</v>
+      </c>
+      <c r="B25" t="s">
+        <v>147</v>
+      </c>
+      <c r="C25" t="s">
+        <v>35</v>
+      </c>
+      <c r="D25" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25">
         <v>1</v>
       </c>
     </row>
@@ -1416,7 +1524,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1566,8 +1674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1575,7 +1683,7 @@
     <col min="1" max="1" width="28.33203125" customWidth="1"/>
     <col min="2" max="2" width="30.83203125" customWidth="1"/>
     <col min="3" max="3" width="32.33203125" customWidth="1"/>
-    <col min="4" max="5" width="33" customWidth="1"/>
+    <col min="4" max="4" width="33" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -1589,10 +1697,10 @@
         <v>91</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>106</v>
+        <v>148</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>117</v>
+        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -1727,10 +1835,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:A13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1791,6 +1899,16 @@
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -1804,118 +1922,108 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8023469F-76F5-624D-BF66-0A486118095E}">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection sqref="A1:D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B03F9D6-05FA-864A-B0C5-D8AE08309FFE}">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29.83203125" customWidth="1"/>
-    <col min="2" max="2" width="27.1640625" customWidth="1"/>
-    <col min="3" max="3" width="28.83203125" customWidth="1"/>
-    <col min="4" max="4" width="34.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>113</v>
-      </c>
-      <c r="B1" t="s">
-        <v>114</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>107</v>
-      </c>
-      <c r="B2" t="s">
-        <v>110</v>
-      </c>
-      <c r="C2" t="s">
-        <v>110</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>108</v>
-      </c>
-      <c r="B3" t="s">
-        <v>111</v>
-      </c>
-      <c r="C3" t="s">
-        <v>111</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>109</v>
-      </c>
-      <c r="B4" t="s">
-        <v>112</v>
-      </c>
-      <c r="C4" t="s">
-        <v>112</v>
-      </c>
-      <c r="D4">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E595DE6E-CBA1-634A-B045-38D514B9DB87}">
-  <dimension ref="A1:C11"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="36" customWidth="1"/>
-    <col min="2" max="2" width="22.33203125" customWidth="1"/>
+    <col min="1" max="1" width="30" customWidth="1"/>
+    <col min="2" max="2" width="22.83203125" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="B1" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="C1" t="s">
-        <v>138</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="B2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -1923,10 +2031,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="B3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -1934,10 +2042,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="B4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -1945,7 +2053,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="B5" t="s">
         <v>131</v>
@@ -1956,10 +2064,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="B6" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -1967,10 +2075,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>123</v>
+        <v>134</v>
       </c>
       <c r="B7" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -1978,10 +2086,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>124</v>
+        <v>136</v>
       </c>
       <c r="B8" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -1989,10 +2097,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>125</v>
+        <v>138</v>
       </c>
       <c r="B9" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -2000,10 +2108,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>126</v>
+        <v>140</v>
       </c>
       <c r="B10" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -2011,10 +2119,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="B11" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="C11">
         <v>1</v>

</xml_diff>

<commit_message>
Added new unit_categories and a new sheet
</commit_message>
<xml_diff>
--- a/lsh_data_processing/lsh_coding.xlsx
+++ b/lsh_data_processing/lsh_coding.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rjs/projects/covid/BCS/lsh_data_processing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{368F3BB7-1505-2F4F-8D0B-D2138D085D8B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A502FFD8-D7E7-0F40-BFB1-30DD35ADA54E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3040" yWindow="-19740" windowWidth="25040" windowHeight="14000" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10260" yWindow="-20300" windowWidth="25040" windowHeight="14000" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="lsh_covid_groups" sheetId="3" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="152">
   <si>
     <t>text_out_category_raw</t>
   </si>
@@ -482,6 +482,12 @@
   </si>
   <si>
     <t>clinical_assessment_category_order_all</t>
+  </si>
+  <si>
+    <t>Fv-G3 BM Göngu</t>
+  </si>
+  <si>
+    <t>Takmörkun meðferðar</t>
   </si>
 </sst>
 </file>
@@ -1069,10 +1075,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView topLeftCell="A8" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1463,10 +1469,10 @@
         <v>144</v>
       </c>
       <c r="B23" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C23" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D23" t="s">
         <v>10</v>
@@ -1506,6 +1512,23 @@
         <v>10</v>
       </c>
       <c r="E25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>150</v>
+      </c>
+      <c r="B26" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D26" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26">
         <v>1</v>
       </c>
     </row>
@@ -1674,7 +1697,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:E8"/>
     </sheetView>
   </sheetViews>
@@ -1835,10 +1858,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:A13"/>
+  <dimension ref="A1:A14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1909,6 +1932,11 @@
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>110</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>151</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update naming convention for lsh data file and adding the most recent lsh coding file
</commit_message>
<xml_diff>
--- a/lsh_data_processing/lsh_coding.xlsx
+++ b/lsh_data_processing/lsh_coding.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rjs/projects/covid/BCS/lsh_data_processing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{368F3BB7-1505-2F4F-8D0B-D2138D085D8B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A502FFD8-D7E7-0F40-BFB1-30DD35ADA54E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3040" yWindow="-19740" windowWidth="25040" windowHeight="14000" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10260" yWindow="-20300" windowWidth="25040" windowHeight="14000" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="lsh_covid_groups" sheetId="3" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="152">
   <si>
     <t>text_out_category_raw</t>
   </si>
@@ -482,6 +482,12 @@
   </si>
   <si>
     <t>clinical_assessment_category_order_all</t>
+  </si>
+  <si>
+    <t>Fv-G3 BM Göngu</t>
+  </si>
+  <si>
+    <t>Takmörkun meðferðar</t>
   </si>
 </sst>
 </file>
@@ -1069,10 +1075,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView topLeftCell="A8" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1463,10 +1469,10 @@
         <v>144</v>
       </c>
       <c r="B23" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C23" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D23" t="s">
         <v>10</v>
@@ -1506,6 +1512,23 @@
         <v>10</v>
       </c>
       <c r="E25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>150</v>
+      </c>
+      <c r="B26" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D26" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26">
         <v>1</v>
       </c>
     </row>
@@ -1674,7 +1697,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:E8"/>
     </sheetView>
   </sheetViews>
@@ -1835,10 +1858,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:A13"/>
+  <dimension ref="A1:A14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1909,6 +1932,11 @@
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>110</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>151</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding support for custom splitting of data set in regard to output tables (not only age_group_simple)
</commit_message>
<xml_diff>
--- a/lsh_data_processing/lsh_coding.xlsx
+++ b/lsh_data_processing/lsh_coding.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10307"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rjs/projects/covid/BCS/lsh_data_processing/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C4EFCE9F-0D8B-C740-9F48-400A2CAC94B9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="27729"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="10260" yWindow="-20300" windowWidth="25040" windowHeight="14000" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14560" firstSheet="4" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="lsh_covid_groups" sheetId="3" r:id="rId1"/>
@@ -23,7 +17,7 @@
     <sheet name="comorbidities" sheetId="8" r:id="rId8"/>
     <sheet name="age_groups" sheetId="9" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="140001"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -33,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="172">
   <si>
     <t>text_out_category_raw</t>
   </si>
@@ -540,12 +534,21 @@
   </si>
   <si>
     <t>51+</t>
+  </si>
+  <si>
+    <t>age_group_order_official</t>
+  </si>
+  <si>
+    <t>age_group_order_three</t>
+  </si>
+  <si>
+    <t>age_group_order_simple</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -628,8 +631,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -654,19 +663,25 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="19">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -725,7 +740,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -777,7 +792,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -971,28 +986,28 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
+    <sheetView topLeftCell="K1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="29.1640625" customWidth="1"/>
     <col min="2" max="2" width="19.83203125" customWidth="1"/>
     <col min="3" max="3" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>37</v>
       </c>
@@ -1003,7 +1018,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
         <v>40</v>
       </c>
@@ -1014,7 +1029,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
         <v>41</v>
       </c>
@@ -1025,7 +1040,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
         <v>42</v>
       </c>
@@ -1036,7 +1051,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
         <v>43</v>
       </c>
@@ -1047,7 +1062,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
         <v>44</v>
       </c>
@@ -1069,21 +1084,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView zoomScale="210" zoomScaleNormal="210" zoomScalePageLayoutView="210" workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="15.1640625" customWidth="1"/>
     <col min="2" max="2" width="16.1640625" customWidth="1"/>
     <col min="3" max="3" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>51</v>
       </c>
@@ -1094,7 +1109,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>54</v>
       </c>
@@ -1105,7 +1120,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>55</v>
       </c>
@@ -1127,14 +1142,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="36.5" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
@@ -1143,7 +1158,7 @@
     <col min="5" max="5" width="25.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -1160,7 +1175,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -1177,7 +1192,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -1194,7 +1209,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -1211,7 +1226,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -1228,7 +1243,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -1245,7 +1260,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -1262,7 +1277,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -1279,7 +1294,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -1296,7 +1311,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -1313,7 +1328,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -1330,7 +1345,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5">
       <c r="A12" s="2" t="s">
         <v>60</v>
       </c>
@@ -1347,7 +1362,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>62</v>
       </c>
@@ -1364,7 +1379,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>63</v>
       </c>
@@ -1381,7 +1396,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5">
       <c r="A15" s="2" t="s">
         <v>64</v>
       </c>
@@ -1398,7 +1413,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5">
       <c r="A16" s="2" t="s">
         <v>65</v>
       </c>
@@ -1415,7 +1430,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5">
       <c r="A17" s="2" t="s">
         <v>66</v>
       </c>
@@ -1432,7 +1447,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5">
       <c r="A18" s="1" t="s">
         <v>85</v>
       </c>
@@ -1449,7 +1464,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>86</v>
       </c>
@@ -1466,7 +1481,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5">
       <c r="A20" s="1" t="s">
         <v>87</v>
       </c>
@@ -1483,7 +1498,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>106</v>
       </c>
@@ -1500,7 +1515,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>107</v>
       </c>
@@ -1517,7 +1532,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
         <v>144</v>
       </c>
@@ -1534,7 +1549,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
         <v>145</v>
       </c>
@@ -1551,7 +1566,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
         <v>146</v>
       </c>
@@ -1568,7 +1583,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
         <v>150</v>
       </c>
@@ -1596,21 +1611,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="31" customWidth="1"/>
     <col min="2" max="2" width="25.1640625" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1624,7 +1639,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1638,7 +1653,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1652,7 +1667,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1666,7 +1681,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1680,7 +1695,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1694,7 +1709,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1708,7 +1723,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -1722,7 +1737,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -1747,14 +1762,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="28.33203125" customWidth="1"/>
     <col min="2" max="2" width="30.83203125" customWidth="1"/>
@@ -1762,7 +1777,7 @@
     <col min="4" max="4" width="33" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>89</v>
       </c>
@@ -1779,7 +1794,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>92</v>
       </c>
@@ -1796,7 +1811,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>93</v>
       </c>
@@ -1813,7 +1828,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>94</v>
       </c>
@@ -1830,7 +1845,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>104</v>
       </c>
@@ -1847,7 +1862,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>95</v>
       </c>
@@ -1864,7 +1879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>96</v>
       </c>
@@ -1881,7 +1896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>97</v>
       </c>
@@ -1910,84 +1925,84 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="24.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1">
       <c r="A3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1">
       <c r="A4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1">
       <c r="A5" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1">
       <c r="A6" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:1">
       <c r="A7" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:1">
       <c r="A8" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:1">
       <c r="A9" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:1">
       <c r="A10" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:1">
       <c r="A11" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:1">
       <c r="A12" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:1">
       <c r="A13" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:1">
       <c r="A14" t="s">
         <v>151</v>
       </c>
@@ -2003,16 +2018,20 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8023469F-76F5-624D-BF66-0A486118095E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="19.33203125" customWidth="1"/>
+    <col min="3" max="3" width="21.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>111</v>
       </c>
@@ -2026,7 +2045,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>115</v>
       </c>
@@ -2040,7 +2059,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>117</v>
       </c>
@@ -2054,7 +2073,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>119</v>
       </c>
@@ -2070,25 +2089,30 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B03F9D6-05FA-864A-B0C5-D8AE08309FFE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="30" customWidth="1"/>
     <col min="2" max="2" width="22.83203125" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>121</v>
       </c>
@@ -2099,7 +2123,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>124</v>
       </c>
@@ -2110,7 +2134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>126</v>
       </c>
@@ -2121,7 +2145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>128</v>
       </c>
@@ -2132,7 +2156,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>130</v>
       </c>
@@ -2143,7 +2167,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>132</v>
       </c>
@@ -2154,7 +2178,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>134</v>
       </c>
@@ -2165,7 +2189,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>136</v>
       </c>
@@ -2176,7 +2200,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>138</v>
       </c>
@@ -2187,7 +2211,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>140</v>
       </c>
@@ -2198,7 +2222,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>142</v>
       </c>
@@ -2211,25 +2235,33 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F50DD301-9CCE-6744-864C-185ECBAFA9CA}">
-  <dimension ref="A1:D122"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G122"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A95" zoomScale="99" workbookViewId="0">
+      <selection activeCell="G53" sqref="G53:G122"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="14.83203125" customWidth="1"/>
     <col min="3" max="3" width="15.5" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
+    <col min="5" max="5" width="21.6640625" customWidth="1"/>
+    <col min="6" max="6" width="20.33203125" customWidth="1"/>
+    <col min="7" max="7" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>152</v>
       </c>
@@ -2242,8 +2274,17 @@
       <c r="D1" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>169</v>
+      </c>
+      <c r="F1" t="s">
+        <v>170</v>
+      </c>
+      <c r="G1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>0</v>
       </c>
@@ -2256,8 +2297,17 @@
       <c r="D2" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2270,8 +2320,17 @@
       <c r="D3" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>2</v>
       </c>
@@ -2284,8 +2343,17 @@
       <c r="D4" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>3</v>
       </c>
@@ -2298,8 +2366,17 @@
       <c r="D5" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>4</v>
       </c>
@@ -2312,8 +2389,17 @@
       <c r="D6" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>5</v>
       </c>
@@ -2326,8 +2412,17 @@
       <c r="D7" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>6</v>
       </c>
@@ -2340,8 +2435,17 @@
       <c r="D8" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>7</v>
       </c>
@@ -2354,8 +2458,17 @@
       <c r="D9" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>8</v>
       </c>
@@ -2368,8 +2481,17 @@
       <c r="D10" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11">
         <v>9</v>
       </c>
@@ -2382,8 +2504,17 @@
       <c r="D11" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12">
         <v>10</v>
       </c>
@@ -2396,8 +2527,17 @@
       <c r="D12" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E12">
+        <v>2</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13">
         <v>11</v>
       </c>
@@ -2410,8 +2550,17 @@
       <c r="D13" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14">
         <v>12</v>
       </c>
@@ -2424,8 +2573,17 @@
       <c r="D14" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E14">
+        <v>2</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15">
         <v>13</v>
       </c>
@@ -2438,8 +2596,17 @@
       <c r="D15" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E15">
+        <v>2</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16">
         <v>14</v>
       </c>
@@ -2452,8 +2619,17 @@
       <c r="D16" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E16">
+        <v>2</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17">
         <v>15</v>
       </c>
@@ -2466,8 +2642,17 @@
       <c r="D17" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E17">
+        <v>2</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18">
         <v>16</v>
       </c>
@@ -2480,8 +2665,17 @@
       <c r="D18" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E18">
+        <v>2</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19">
         <v>17</v>
       </c>
@@ -2494,8 +2688,17 @@
       <c r="D19" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E19">
+        <v>2</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20">
         <v>18</v>
       </c>
@@ -2508,8 +2711,17 @@
       <c r="D20" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E20">
+        <v>2</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21">
         <v>19</v>
       </c>
@@ -2522,8 +2734,17 @@
       <c r="D21" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E21">
+        <v>2</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22">
         <v>20</v>
       </c>
@@ -2536,8 +2757,17 @@
       <c r="D22" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E22">
+        <v>3</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23">
         <v>21</v>
       </c>
@@ -2550,8 +2780,17 @@
       <c r="D23" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E23">
+        <v>3</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24">
         <v>22</v>
       </c>
@@ -2564,8 +2803,17 @@
       <c r="D24" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E24">
+        <v>3</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
       <c r="A25">
         <v>23</v>
       </c>
@@ -2578,8 +2826,17 @@
       <c r="D25" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E25">
+        <v>3</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
       <c r="A26">
         <v>24</v>
       </c>
@@ -2592,8 +2849,17 @@
       <c r="D26" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E26">
+        <v>3</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
       <c r="A27">
         <v>25</v>
       </c>
@@ -2606,8 +2872,17 @@
       <c r="D27" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E27">
+        <v>3</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
       <c r="A28">
         <v>26</v>
       </c>
@@ -2620,8 +2895,17 @@
       <c r="D28" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E28">
+        <v>3</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
       <c r="A29">
         <v>27</v>
       </c>
@@ -2634,8 +2918,17 @@
       <c r="D29" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E29">
+        <v>3</v>
+      </c>
+      <c r="F29">
+        <v>1</v>
+      </c>
+      <c r="G29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
       <c r="A30">
         <v>28</v>
       </c>
@@ -2648,8 +2941,17 @@
       <c r="D30" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E30">
+        <v>3</v>
+      </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
+      <c r="G30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
       <c r="A31">
         <v>29</v>
       </c>
@@ -2662,8 +2964,17 @@
       <c r="D31" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E31">
+        <v>3</v>
+      </c>
+      <c r="F31">
+        <v>1</v>
+      </c>
+      <c r="G31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
       <c r="A32">
         <v>30</v>
       </c>
@@ -2676,8 +2987,17 @@
       <c r="D32" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E32">
+        <v>4</v>
+      </c>
+      <c r="F32">
+        <v>1</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
       <c r="A33">
         <v>31</v>
       </c>
@@ -2690,8 +3010,17 @@
       <c r="D33" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E33">
+        <v>4</v>
+      </c>
+      <c r="F33">
+        <v>1</v>
+      </c>
+      <c r="G33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
       <c r="A34">
         <v>32</v>
       </c>
@@ -2704,8 +3033,17 @@
       <c r="D34" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E34">
+        <v>4</v>
+      </c>
+      <c r="F34">
+        <v>1</v>
+      </c>
+      <c r="G34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
       <c r="A35">
         <v>33</v>
       </c>
@@ -2718,8 +3056,17 @@
       <c r="D35" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E35">
+        <v>4</v>
+      </c>
+      <c r="F35">
+        <v>1</v>
+      </c>
+      <c r="G35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
       <c r="A36">
         <v>34</v>
       </c>
@@ -2732,8 +3079,17 @@
       <c r="D36" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E36">
+        <v>4</v>
+      </c>
+      <c r="F36">
+        <v>1</v>
+      </c>
+      <c r="G36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
       <c r="A37">
         <v>35</v>
       </c>
@@ -2746,8 +3102,17 @@
       <c r="D37" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E37">
+        <v>4</v>
+      </c>
+      <c r="F37">
+        <v>1</v>
+      </c>
+      <c r="G37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
       <c r="A38">
         <v>36</v>
       </c>
@@ -2760,8 +3125,17 @@
       <c r="D38" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E38">
+        <v>4</v>
+      </c>
+      <c r="F38">
+        <v>1</v>
+      </c>
+      <c r="G38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
       <c r="A39">
         <v>37</v>
       </c>
@@ -2774,8 +3148,17 @@
       <c r="D39" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E39">
+        <v>4</v>
+      </c>
+      <c r="F39">
+        <v>1</v>
+      </c>
+      <c r="G39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
       <c r="A40">
         <v>38</v>
       </c>
@@ -2788,8 +3171,17 @@
       <c r="D40" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E40">
+        <v>4</v>
+      </c>
+      <c r="F40">
+        <v>1</v>
+      </c>
+      <c r="G40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
       <c r="A41">
         <v>39</v>
       </c>
@@ -2802,8 +3194,17 @@
       <c r="D41" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E41">
+        <v>4</v>
+      </c>
+      <c r="F41">
+        <v>1</v>
+      </c>
+      <c r="G41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
       <c r="A42">
         <v>40</v>
       </c>
@@ -2816,8 +3217,17 @@
       <c r="D42" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E42">
+        <v>5</v>
+      </c>
+      <c r="F42">
+        <v>1</v>
+      </c>
+      <c r="G42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
       <c r="A43">
         <v>41</v>
       </c>
@@ -2830,8 +3240,17 @@
       <c r="D43" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E43">
+        <v>5</v>
+      </c>
+      <c r="F43">
+        <v>1</v>
+      </c>
+      <c r="G43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
       <c r="A44">
         <v>42</v>
       </c>
@@ -2844,8 +3263,17 @@
       <c r="D44" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E44">
+        <v>5</v>
+      </c>
+      <c r="F44">
+        <v>1</v>
+      </c>
+      <c r="G44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
       <c r="A45">
         <v>43</v>
       </c>
@@ -2858,8 +3286,17 @@
       <c r="D45" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E45">
+        <v>5</v>
+      </c>
+      <c r="F45">
+        <v>1</v>
+      </c>
+      <c r="G45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
       <c r="A46">
         <v>44</v>
       </c>
@@ -2872,8 +3309,17 @@
       <c r="D46" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E46">
+        <v>5</v>
+      </c>
+      <c r="F46">
+        <v>1</v>
+      </c>
+      <c r="G46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
       <c r="A47">
         <v>45</v>
       </c>
@@ -2886,8 +3332,17 @@
       <c r="D47" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E47">
+        <v>5</v>
+      </c>
+      <c r="F47">
+        <v>1</v>
+      </c>
+      <c r="G47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
       <c r="A48">
         <v>46</v>
       </c>
@@ -2900,8 +3355,17 @@
       <c r="D48" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E48">
+        <v>5</v>
+      </c>
+      <c r="F48">
+        <v>1</v>
+      </c>
+      <c r="G48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
       <c r="A49">
         <v>47</v>
       </c>
@@ -2914,8 +3378,17 @@
       <c r="D49" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E49">
+        <v>5</v>
+      </c>
+      <c r="F49">
+        <v>1</v>
+      </c>
+      <c r="G49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
       <c r="A50">
         <v>48</v>
       </c>
@@ -2928,8 +3401,17 @@
       <c r="D50" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E50">
+        <v>5</v>
+      </c>
+      <c r="F50">
+        <v>1</v>
+      </c>
+      <c r="G50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
       <c r="A51">
         <v>49</v>
       </c>
@@ -2942,8 +3424,17 @@
       <c r="D51" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E51">
+        <v>5</v>
+      </c>
+      <c r="F51">
+        <v>1</v>
+      </c>
+      <c r="G51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
       <c r="A52">
         <v>50</v>
       </c>
@@ -2956,8 +3447,17 @@
       <c r="D52" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E52">
+        <v>6</v>
+      </c>
+      <c r="F52">
+        <v>1</v>
+      </c>
+      <c r="G52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
       <c r="A53">
         <v>51</v>
       </c>
@@ -2970,8 +3470,17 @@
       <c r="D53" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E53">
+        <v>6</v>
+      </c>
+      <c r="F53">
+        <v>2</v>
+      </c>
+      <c r="G53">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
       <c r="A54">
         <v>52</v>
       </c>
@@ -2984,8 +3493,17 @@
       <c r="D54" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E54">
+        <v>6</v>
+      </c>
+      <c r="F54">
+        <v>2</v>
+      </c>
+      <c r="G54">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
       <c r="A55">
         <v>53</v>
       </c>
@@ -2998,8 +3516,17 @@
       <c r="D55" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E55">
+        <v>6</v>
+      </c>
+      <c r="F55">
+        <v>2</v>
+      </c>
+      <c r="G55">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
       <c r="A56">
         <v>54</v>
       </c>
@@ -3012,8 +3539,17 @@
       <c r="D56" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E56">
+        <v>6</v>
+      </c>
+      <c r="F56">
+        <v>2</v>
+      </c>
+      <c r="G56">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
       <c r="A57">
         <v>55</v>
       </c>
@@ -3026,8 +3562,17 @@
       <c r="D57" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E57">
+        <v>6</v>
+      </c>
+      <c r="F57">
+        <v>2</v>
+      </c>
+      <c r="G57">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
       <c r="A58">
         <v>56</v>
       </c>
@@ -3040,8 +3585,17 @@
       <c r="D58" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E58">
+        <v>6</v>
+      </c>
+      <c r="F58">
+        <v>2</v>
+      </c>
+      <c r="G58">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
       <c r="A59">
         <v>57</v>
       </c>
@@ -3054,8 +3608,17 @@
       <c r="D59" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E59">
+        <v>6</v>
+      </c>
+      <c r="F59">
+        <v>2</v>
+      </c>
+      <c r="G59">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
       <c r="A60">
         <v>58</v>
       </c>
@@ -3068,8 +3631,17 @@
       <c r="D60" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E60">
+        <v>6</v>
+      </c>
+      <c r="F60">
+        <v>2</v>
+      </c>
+      <c r="G60">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
       <c r="A61">
         <v>59</v>
       </c>
@@ -3082,8 +3654,17 @@
       <c r="D61" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E61">
+        <v>6</v>
+      </c>
+      <c r="F61">
+        <v>2</v>
+      </c>
+      <c r="G61">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
       <c r="A62">
         <v>60</v>
       </c>
@@ -3096,8 +3677,17 @@
       <c r="D62" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E62">
+        <v>7</v>
+      </c>
+      <c r="F62">
+        <v>2</v>
+      </c>
+      <c r="G62">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
       <c r="A63">
         <v>61</v>
       </c>
@@ -3110,8 +3700,17 @@
       <c r="D63" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E63">
+        <v>7</v>
+      </c>
+      <c r="F63">
+        <v>2</v>
+      </c>
+      <c r="G63">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
       <c r="A64">
         <v>62</v>
       </c>
@@ -3124,8 +3723,17 @@
       <c r="D64" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E64">
+        <v>7</v>
+      </c>
+      <c r="F64">
+        <v>2</v>
+      </c>
+      <c r="G64">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7">
       <c r="A65">
         <v>63</v>
       </c>
@@ -3138,8 +3746,17 @@
       <c r="D65" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E65">
+        <v>7</v>
+      </c>
+      <c r="F65">
+        <v>2</v>
+      </c>
+      <c r="G65">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7">
       <c r="A66">
         <v>64</v>
       </c>
@@ -3152,8 +3769,17 @@
       <c r="D66" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E66">
+        <v>7</v>
+      </c>
+      <c r="F66">
+        <v>2</v>
+      </c>
+      <c r="G66">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7">
       <c r="A67">
         <v>65</v>
       </c>
@@ -3166,8 +3792,17 @@
       <c r="D67" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E67">
+        <v>7</v>
+      </c>
+      <c r="F67">
+        <v>2</v>
+      </c>
+      <c r="G67">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7">
       <c r="A68">
         <v>66</v>
       </c>
@@ -3180,8 +3815,17 @@
       <c r="D68" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E68">
+        <v>7</v>
+      </c>
+      <c r="F68">
+        <v>2</v>
+      </c>
+      <c r="G68">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7">
       <c r="A69">
         <v>67</v>
       </c>
@@ -3194,8 +3838,17 @@
       <c r="D69" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E69">
+        <v>7</v>
+      </c>
+      <c r="F69">
+        <v>2</v>
+      </c>
+      <c r="G69">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7">
       <c r="A70">
         <v>68</v>
       </c>
@@ -3208,8 +3861,17 @@
       <c r="D70" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E70">
+        <v>7</v>
+      </c>
+      <c r="F70">
+        <v>2</v>
+      </c>
+      <c r="G70">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7">
       <c r="A71">
         <v>69</v>
       </c>
@@ -3222,8 +3884,17 @@
       <c r="D71" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E71">
+        <v>7</v>
+      </c>
+      <c r="F71">
+        <v>2</v>
+      </c>
+      <c r="G71">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7">
       <c r="A72">
         <v>70</v>
       </c>
@@ -3236,8 +3907,17 @@
       <c r="D72" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E72">
+        <v>8</v>
+      </c>
+      <c r="F72">
+        <v>2</v>
+      </c>
+      <c r="G72">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7">
       <c r="A73">
         <v>71</v>
       </c>
@@ -3250,8 +3930,17 @@
       <c r="D73" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E73">
+        <v>8</v>
+      </c>
+      <c r="F73">
+        <v>2</v>
+      </c>
+      <c r="G73">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7">
       <c r="A74">
         <v>72</v>
       </c>
@@ -3264,8 +3953,17 @@
       <c r="D74" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E74">
+        <v>8</v>
+      </c>
+      <c r="F74">
+        <v>2</v>
+      </c>
+      <c r="G74">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7">
       <c r="A75">
         <v>73</v>
       </c>
@@ -3278,8 +3976,17 @@
       <c r="D75" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E75">
+        <v>8</v>
+      </c>
+      <c r="F75">
+        <v>2</v>
+      </c>
+      <c r="G75">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7">
       <c r="A76">
         <v>74</v>
       </c>
@@ -3292,8 +3999,17 @@
       <c r="D76" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E76">
+        <v>8</v>
+      </c>
+      <c r="F76">
+        <v>2</v>
+      </c>
+      <c r="G76">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7">
       <c r="A77">
         <v>75</v>
       </c>
@@ -3306,8 +4022,17 @@
       <c r="D77" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E77">
+        <v>8</v>
+      </c>
+      <c r="F77">
+        <v>3</v>
+      </c>
+      <c r="G77">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7">
       <c r="A78">
         <v>76</v>
       </c>
@@ -3320,8 +4045,17 @@
       <c r="D78" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E78">
+        <v>8</v>
+      </c>
+      <c r="F78">
+        <v>3</v>
+      </c>
+      <c r="G78">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7">
       <c r="A79">
         <v>77</v>
       </c>
@@ -3334,8 +4068,17 @@
       <c r="D79" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E79">
+        <v>8</v>
+      </c>
+      <c r="F79">
+        <v>3</v>
+      </c>
+      <c r="G79">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7">
       <c r="A80">
         <v>78</v>
       </c>
@@ -3348,8 +4091,17 @@
       <c r="D80" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E80">
+        <v>8</v>
+      </c>
+      <c r="F80">
+        <v>3</v>
+      </c>
+      <c r="G80">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7">
       <c r="A81">
         <v>79</v>
       </c>
@@ -3362,8 +4114,17 @@
       <c r="D81" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E81">
+        <v>8</v>
+      </c>
+      <c r="F81">
+        <v>3</v>
+      </c>
+      <c r="G81">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7">
       <c r="A82">
         <v>80</v>
       </c>
@@ -3376,8 +4137,17 @@
       <c r="D82" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E82">
+        <v>9</v>
+      </c>
+      <c r="F82">
+        <v>3</v>
+      </c>
+      <c r="G82">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7">
       <c r="A83">
         <v>81</v>
       </c>
@@ -3390,8 +4160,17 @@
       <c r="D83" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E83">
+        <v>9</v>
+      </c>
+      <c r="F83">
+        <v>3</v>
+      </c>
+      <c r="G83">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7">
       <c r="A84">
         <v>82</v>
       </c>
@@ -3404,8 +4183,17 @@
       <c r="D84" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E84">
+        <v>9</v>
+      </c>
+      <c r="F84">
+        <v>3</v>
+      </c>
+      <c r="G84">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7">
       <c r="A85">
         <v>83</v>
       </c>
@@ -3418,8 +4206,17 @@
       <c r="D85" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E85">
+        <v>9</v>
+      </c>
+      <c r="F85">
+        <v>3</v>
+      </c>
+      <c r="G85">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7">
       <c r="A86">
         <v>84</v>
       </c>
@@ -3432,8 +4229,17 @@
       <c r="D86" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E86">
+        <v>9</v>
+      </c>
+      <c r="F86">
+        <v>3</v>
+      </c>
+      <c r="G86">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7">
       <c r="A87">
         <v>85</v>
       </c>
@@ -3446,8 +4252,17 @@
       <c r="D87" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E87">
+        <v>9</v>
+      </c>
+      <c r="F87">
+        <v>3</v>
+      </c>
+      <c r="G87">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7">
       <c r="A88">
         <v>86</v>
       </c>
@@ -3460,8 +4275,17 @@
       <c r="D88" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E88">
+        <v>9</v>
+      </c>
+      <c r="F88">
+        <v>3</v>
+      </c>
+      <c r="G88">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7">
       <c r="A89">
         <v>87</v>
       </c>
@@ -3474,8 +4298,17 @@
       <c r="D89" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E89">
+        <v>9</v>
+      </c>
+      <c r="F89">
+        <v>3</v>
+      </c>
+      <c r="G89">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7">
       <c r="A90">
         <v>88</v>
       </c>
@@ -3488,8 +4321,17 @@
       <c r="D90" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E90">
+        <v>9</v>
+      </c>
+      <c r="F90">
+        <v>3</v>
+      </c>
+      <c r="G90">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7">
       <c r="A91">
         <v>89</v>
       </c>
@@ -3502,8 +4344,17 @@
       <c r="D91" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E91">
+        <v>9</v>
+      </c>
+      <c r="F91">
+        <v>3</v>
+      </c>
+      <c r="G91">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7">
       <c r="A92">
         <v>90</v>
       </c>
@@ -3516,8 +4367,17 @@
       <c r="D92" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E92">
+        <v>9</v>
+      </c>
+      <c r="F92">
+        <v>3</v>
+      </c>
+      <c r="G92">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7">
       <c r="A93">
         <v>91</v>
       </c>
@@ -3530,8 +4390,17 @@
       <c r="D93" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E93">
+        <v>9</v>
+      </c>
+      <c r="F93">
+        <v>3</v>
+      </c>
+      <c r="G93">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7">
       <c r="A94">
         <v>92</v>
       </c>
@@ -3544,8 +4413,17 @@
       <c r="D94" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E94">
+        <v>9</v>
+      </c>
+      <c r="F94">
+        <v>3</v>
+      </c>
+      <c r="G94">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7">
       <c r="A95">
         <v>93</v>
       </c>
@@ -3558,8 +4436,17 @@
       <c r="D95" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E95">
+        <v>9</v>
+      </c>
+      <c r="F95">
+        <v>3</v>
+      </c>
+      <c r="G95">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7">
       <c r="A96">
         <v>94</v>
       </c>
@@ -3572,8 +4459,17 @@
       <c r="D96" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E96">
+        <v>9</v>
+      </c>
+      <c r="F96">
+        <v>3</v>
+      </c>
+      <c r="G96">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7">
       <c r="A97">
         <v>95</v>
       </c>
@@ -3586,8 +4482,17 @@
       <c r="D97" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E97">
+        <v>9</v>
+      </c>
+      <c r="F97">
+        <v>3</v>
+      </c>
+      <c r="G97">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7">
       <c r="A98">
         <v>96</v>
       </c>
@@ -3600,8 +4505,17 @@
       <c r="D98" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E98">
+        <v>9</v>
+      </c>
+      <c r="F98">
+        <v>3</v>
+      </c>
+      <c r="G98">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7">
       <c r="A99">
         <v>97</v>
       </c>
@@ -3614,8 +4528,17 @@
       <c r="D99" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E99">
+        <v>9</v>
+      </c>
+      <c r="F99">
+        <v>3</v>
+      </c>
+      <c r="G99">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7">
       <c r="A100">
         <v>98</v>
       </c>
@@ -3628,8 +4551,17 @@
       <c r="D100" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E100">
+        <v>9</v>
+      </c>
+      <c r="F100">
+        <v>3</v>
+      </c>
+      <c r="G100">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7">
       <c r="A101">
         <v>99</v>
       </c>
@@ -3642,8 +4574,17 @@
       <c r="D101" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E101">
+        <v>9</v>
+      </c>
+      <c r="F101">
+        <v>3</v>
+      </c>
+      <c r="G101">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7">
       <c r="A102">
         <v>100</v>
       </c>
@@ -3656,8 +4597,17 @@
       <c r="D102" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E102">
+        <v>9</v>
+      </c>
+      <c r="F102">
+        <v>3</v>
+      </c>
+      <c r="G102">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7">
       <c r="A103">
         <v>101</v>
       </c>
@@ -3670,8 +4620,17 @@
       <c r="D103" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E103">
+        <v>9</v>
+      </c>
+      <c r="F103">
+        <v>3</v>
+      </c>
+      <c r="G103">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7">
       <c r="A104">
         <v>102</v>
       </c>
@@ -3684,8 +4643,17 @@
       <c r="D104" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E104">
+        <v>9</v>
+      </c>
+      <c r="F104">
+        <v>3</v>
+      </c>
+      <c r="G104">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7">
       <c r="A105">
         <v>103</v>
       </c>
@@ -3698,8 +4666,17 @@
       <c r="D105" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E105">
+        <v>9</v>
+      </c>
+      <c r="F105">
+        <v>3</v>
+      </c>
+      <c r="G105">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7">
       <c r="A106">
         <v>104</v>
       </c>
@@ -3712,8 +4689,17 @@
       <c r="D106" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E106">
+        <v>9</v>
+      </c>
+      <c r="F106">
+        <v>3</v>
+      </c>
+      <c r="G106">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7">
       <c r="A107">
         <v>105</v>
       </c>
@@ -3726,8 +4712,17 @@
       <c r="D107" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E107">
+        <v>9</v>
+      </c>
+      <c r="F107">
+        <v>3</v>
+      </c>
+      <c r="G107">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7">
       <c r="A108">
         <v>106</v>
       </c>
@@ -3740,8 +4735,17 @@
       <c r="D108" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E108">
+        <v>9</v>
+      </c>
+      <c r="F108">
+        <v>3</v>
+      </c>
+      <c r="G108">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7">
       <c r="A109">
         <v>107</v>
       </c>
@@ -3754,8 +4758,17 @@
       <c r="D109" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E109">
+        <v>9</v>
+      </c>
+      <c r="F109">
+        <v>3</v>
+      </c>
+      <c r="G109">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7">
       <c r="A110">
         <v>108</v>
       </c>
@@ -3768,8 +4781,17 @@
       <c r="D110" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E110">
+        <v>9</v>
+      </c>
+      <c r="F110">
+        <v>3</v>
+      </c>
+      <c r="G110">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7">
       <c r="A111">
         <v>109</v>
       </c>
@@ -3782,8 +4804,17 @@
       <c r="D111" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E111">
+        <v>9</v>
+      </c>
+      <c r="F111">
+        <v>3</v>
+      </c>
+      <c r="G111">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7">
       <c r="A112">
         <v>110</v>
       </c>
@@ -3796,8 +4827,17 @@
       <c r="D112" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E112">
+        <v>9</v>
+      </c>
+      <c r="F112">
+        <v>3</v>
+      </c>
+      <c r="G112">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7">
       <c r="A113">
         <v>111</v>
       </c>
@@ -3810,8 +4850,17 @@
       <c r="D113" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E113">
+        <v>9</v>
+      </c>
+      <c r="F113">
+        <v>3</v>
+      </c>
+      <c r="G113">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7">
       <c r="A114">
         <v>112</v>
       </c>
@@ -3824,8 +4873,17 @@
       <c r="D114" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E114">
+        <v>9</v>
+      </c>
+      <c r="F114">
+        <v>3</v>
+      </c>
+      <c r="G114">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7">
       <c r="A115">
         <v>113</v>
       </c>
@@ -3838,8 +4896,17 @@
       <c r="D115" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E115">
+        <v>9</v>
+      </c>
+      <c r="F115">
+        <v>3</v>
+      </c>
+      <c r="G115">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7">
       <c r="A116">
         <v>114</v>
       </c>
@@ -3852,8 +4919,17 @@
       <c r="D116" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E116">
+        <v>9</v>
+      </c>
+      <c r="F116">
+        <v>3</v>
+      </c>
+      <c r="G116">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7">
       <c r="A117">
         <v>115</v>
       </c>
@@ -3866,8 +4942,17 @@
       <c r="D117" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E117">
+        <v>9</v>
+      </c>
+      <c r="F117">
+        <v>3</v>
+      </c>
+      <c r="G117">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7">
       <c r="A118">
         <v>116</v>
       </c>
@@ -3880,8 +4965,17 @@
       <c r="D118" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E118">
+        <v>9</v>
+      </c>
+      <c r="F118">
+        <v>3</v>
+      </c>
+      <c r="G118">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7">
       <c r="A119">
         <v>117</v>
       </c>
@@ -3894,8 +4988,17 @@
       <c r="D119" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E119">
+        <v>9</v>
+      </c>
+      <c r="F119">
+        <v>3</v>
+      </c>
+      <c r="G119">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7">
       <c r="A120">
         <v>118</v>
       </c>
@@ -3908,8 +5011,17 @@
       <c r="D120" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E120">
+        <v>9</v>
+      </c>
+      <c r="F120">
+        <v>3</v>
+      </c>
+      <c r="G120">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7">
       <c r="A121">
         <v>119</v>
       </c>
@@ -3922,8 +5034,17 @@
       <c r="D121" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E121">
+        <v>9</v>
+      </c>
+      <c r="F121">
+        <v>3</v>
+      </c>
+      <c r="G121">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7">
       <c r="A122">
         <v>120</v>
       </c>
@@ -3936,8 +5057,23 @@
       <c r="D122" s="4" t="s">
         <v>168</v>
       </c>
+      <c r="E122">
+        <v>9</v>
+      </c>
+      <c r="F122">
+        <v>3</v>
+      </c>
+      <c r="G122">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added new unit category and new sheet
</commit_message>
<xml_diff>
--- a/lsh_data_processing/lsh_coding.xlsx
+++ b/lsh_data_processing/lsh_coding.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rjs/projects/covid/BCS/lsh_data_processing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C4EFCE9F-0D8B-C740-9F48-400A2CAC94B9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B5CE09B-61A6-5840-8364-5D4617DC6666}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10260" yWindow="-20300" windowWidth="25040" windowHeight="14000" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4740" yWindow="-20380" windowWidth="25040" windowHeight="14000" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="lsh_covid_groups" sheetId="3" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="171">
   <si>
     <t>text_out_category_raw</t>
   </si>
@@ -540,6 +540,12 @@
   </si>
   <si>
     <t>51+</t>
+  </si>
+  <si>
+    <t>Hb-23B BM Fæðingarvakt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GD Birkiborg-form </t>
   </si>
 </sst>
 </file>
@@ -1128,10 +1134,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView topLeftCell="B11" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1582,6 +1588,23 @@
         <v>10</v>
       </c>
       <c r="E26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>169</v>
+      </c>
+      <c r="B27" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27" t="s">
+        <v>33</v>
+      </c>
+      <c r="D27" t="s">
+        <v>10</v>
+      </c>
+      <c r="E27">
         <v>1</v>
       </c>
     </row>
@@ -1911,10 +1934,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:A14"/>
+  <dimension ref="A1:A15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1990,6 +2013,11 @@
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>151</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -2218,7 +2246,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F50DD301-9CCE-6744-864C-185ECBAFA9CA}">
   <dimension ref="A1:D122"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
+    <sheetView zoomScale="99" workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fixes to get the new merge to run
</commit_message>
<xml_diff>
--- a/lsh_data_processing/lsh_coding.xlsx
+++ b/lsh_data_processing/lsh_coding.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rjs/projects/covid/BCS/lsh_data_processing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B5CE09B-61A6-5840-8364-5D4617DC6666}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3091E55-57DF-F94D-A332-B53C3306A2A3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4740" yWindow="-20380" windowWidth="25040" windowHeight="14000" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4740" yWindow="-20380" windowWidth="25040" windowHeight="14000" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="lsh_covid_groups" sheetId="3" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="174">
   <si>
     <t>text_out_category_raw</t>
   </si>
@@ -546,6 +546,15 @@
   </si>
   <si>
     <t xml:space="preserve">GD Birkiborg-form </t>
+  </si>
+  <si>
+    <t>age_group_order_official</t>
+  </si>
+  <si>
+    <t>age_group_order_three</t>
+  </si>
+  <si>
+    <t>age_group_order_simple</t>
   </si>
 </sst>
 </file>
@@ -1936,7 +1945,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:A15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
@@ -2244,10 +2253,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F50DD301-9CCE-6744-864C-185ECBAFA9CA}">
-  <dimension ref="A1:D122"/>
+  <dimension ref="A1:G122"/>
   <sheetViews>
-    <sheetView zoomScale="99" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2257,7 +2266,7 @@
     <col min="4" max="4" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>152</v>
       </c>
@@ -2270,8 +2279,17 @@
       <c r="D1" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>171</v>
+      </c>
+      <c r="F1" t="s">
+        <v>172</v>
+      </c>
+      <c r="G1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -2284,8 +2302,17 @@
       <c r="D2" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2298,8 +2325,17 @@
       <c r="D3" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -2312,8 +2348,17 @@
       <c r="D4" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -2326,8 +2371,17 @@
       <c r="D5" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -2340,8 +2394,17 @@
       <c r="D6" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -2354,8 +2417,17 @@
       <c r="D7" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -2368,8 +2440,17 @@
       <c r="D8" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
@@ -2382,8 +2463,17 @@
       <c r="D9" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
@@ -2396,8 +2486,17 @@
       <c r="D10" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
@@ -2410,8 +2509,17 @@
       <c r="D11" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
@@ -2424,8 +2532,17 @@
       <c r="D12" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E12">
+        <v>2</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11</v>
       </c>
@@ -2438,8 +2555,17 @@
       <c r="D13" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>12</v>
       </c>
@@ -2452,8 +2578,17 @@
       <c r="D14" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E14">
+        <v>2</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>13</v>
       </c>
@@ -2466,8 +2601,17 @@
       <c r="D15" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E15">
+        <v>2</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>14</v>
       </c>
@@ -2480,8 +2624,17 @@
       <c r="D16" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E16">
+        <v>2</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>15</v>
       </c>
@@ -2494,8 +2647,17 @@
       <c r="D17" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E17">
+        <v>2</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>16</v>
       </c>
@@ -2508,8 +2670,17 @@
       <c r="D18" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E18">
+        <v>2</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>17</v>
       </c>
@@ -2522,8 +2693,17 @@
       <c r="D19" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E19">
+        <v>2</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>18</v>
       </c>
@@ -2536,8 +2716,17 @@
       <c r="D20" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E20">
+        <v>2</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>19</v>
       </c>
@@ -2550,8 +2739,17 @@
       <c r="D21" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E21">
+        <v>2</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>20</v>
       </c>
@@ -2564,8 +2762,17 @@
       <c r="D22" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E22">
+        <v>3</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>21</v>
       </c>
@@ -2578,8 +2785,17 @@
       <c r="D23" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E23">
+        <v>3</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>22</v>
       </c>
@@ -2592,8 +2808,17 @@
       <c r="D24" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E24">
+        <v>3</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>23</v>
       </c>
@@ -2606,8 +2831,17 @@
       <c r="D25" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E25">
+        <v>3</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>24</v>
       </c>
@@ -2620,8 +2854,17 @@
       <c r="D26" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E26">
+        <v>3</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>25</v>
       </c>
@@ -2634,8 +2877,17 @@
       <c r="D27" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E27">
+        <v>3</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>26</v>
       </c>
@@ -2648,8 +2900,17 @@
       <c r="D28" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E28">
+        <v>3</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>27</v>
       </c>
@@ -2662,8 +2923,17 @@
       <c r="D29" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E29">
+        <v>3</v>
+      </c>
+      <c r="F29">
+        <v>1</v>
+      </c>
+      <c r="G29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>28</v>
       </c>
@@ -2676,8 +2946,17 @@
       <c r="D30" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E30">
+        <v>3</v>
+      </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
+      <c r="G30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>29</v>
       </c>
@@ -2690,8 +2969,17 @@
       <c r="D31" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E31">
+        <v>3</v>
+      </c>
+      <c r="F31">
+        <v>1</v>
+      </c>
+      <c r="G31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>30</v>
       </c>
@@ -2704,8 +2992,17 @@
       <c r="D32" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E32">
+        <v>4</v>
+      </c>
+      <c r="F32">
+        <v>1</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>31</v>
       </c>
@@ -2718,8 +3015,17 @@
       <c r="D33" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E33">
+        <v>4</v>
+      </c>
+      <c r="F33">
+        <v>1</v>
+      </c>
+      <c r="G33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>32</v>
       </c>
@@ -2732,8 +3038,17 @@
       <c r="D34" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E34">
+        <v>4</v>
+      </c>
+      <c r="F34">
+        <v>1</v>
+      </c>
+      <c r="G34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>33</v>
       </c>
@@ -2746,8 +3061,17 @@
       <c r="D35" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E35">
+        <v>4</v>
+      </c>
+      <c r="F35">
+        <v>1</v>
+      </c>
+      <c r="G35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>34</v>
       </c>
@@ -2760,8 +3084,17 @@
       <c r="D36" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E36">
+        <v>4</v>
+      </c>
+      <c r="F36">
+        <v>1</v>
+      </c>
+      <c r="G36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>35</v>
       </c>
@@ -2774,8 +3107,17 @@
       <c r="D37" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E37">
+        <v>4</v>
+      </c>
+      <c r="F37">
+        <v>1</v>
+      </c>
+      <c r="G37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>36</v>
       </c>
@@ -2788,8 +3130,17 @@
       <c r="D38" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E38">
+        <v>4</v>
+      </c>
+      <c r="F38">
+        <v>1</v>
+      </c>
+      <c r="G38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>37</v>
       </c>
@@ -2802,8 +3153,17 @@
       <c r="D39" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E39">
+        <v>4</v>
+      </c>
+      <c r="F39">
+        <v>1</v>
+      </c>
+      <c r="G39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>38</v>
       </c>
@@ -2816,8 +3176,17 @@
       <c r="D40" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E40">
+        <v>4</v>
+      </c>
+      <c r="F40">
+        <v>1</v>
+      </c>
+      <c r="G40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>39</v>
       </c>
@@ -2830,8 +3199,17 @@
       <c r="D41" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E41">
+        <v>4</v>
+      </c>
+      <c r="F41">
+        <v>1</v>
+      </c>
+      <c r="G41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>40</v>
       </c>
@@ -2844,8 +3222,17 @@
       <c r="D42" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E42">
+        <v>5</v>
+      </c>
+      <c r="F42">
+        <v>1</v>
+      </c>
+      <c r="G42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>41</v>
       </c>
@@ -2858,8 +3245,17 @@
       <c r="D43" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E43">
+        <v>5</v>
+      </c>
+      <c r="F43">
+        <v>1</v>
+      </c>
+      <c r="G43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>42</v>
       </c>
@@ -2872,8 +3268,17 @@
       <c r="D44" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E44">
+        <v>5</v>
+      </c>
+      <c r="F44">
+        <v>1</v>
+      </c>
+      <c r="G44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>43</v>
       </c>
@@ -2886,8 +3291,17 @@
       <c r="D45" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E45">
+        <v>5</v>
+      </c>
+      <c r="F45">
+        <v>1</v>
+      </c>
+      <c r="G45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>44</v>
       </c>
@@ -2900,8 +3314,17 @@
       <c r="D46" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E46">
+        <v>5</v>
+      </c>
+      <c r="F46">
+        <v>1</v>
+      </c>
+      <c r="G46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>45</v>
       </c>
@@ -2914,8 +3337,17 @@
       <c r="D47" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E47">
+        <v>5</v>
+      </c>
+      <c r="F47">
+        <v>1</v>
+      </c>
+      <c r="G47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>46</v>
       </c>
@@ -2928,8 +3360,17 @@
       <c r="D48" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E48">
+        <v>5</v>
+      </c>
+      <c r="F48">
+        <v>1</v>
+      </c>
+      <c r="G48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>47</v>
       </c>
@@ -2942,8 +3383,17 @@
       <c r="D49" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E49">
+        <v>5</v>
+      </c>
+      <c r="F49">
+        <v>1</v>
+      </c>
+      <c r="G49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>48</v>
       </c>
@@ -2956,8 +3406,17 @@
       <c r="D50" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E50">
+        <v>5</v>
+      </c>
+      <c r="F50">
+        <v>1</v>
+      </c>
+      <c r="G50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>49</v>
       </c>
@@ -2970,8 +3429,17 @@
       <c r="D51" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E51">
+        <v>5</v>
+      </c>
+      <c r="F51">
+        <v>1</v>
+      </c>
+      <c r="G51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>50</v>
       </c>
@@ -2984,8 +3452,17 @@
       <c r="D52" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E52">
+        <v>6</v>
+      </c>
+      <c r="F52">
+        <v>1</v>
+      </c>
+      <c r="G52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>51</v>
       </c>
@@ -2998,8 +3475,17 @@
       <c r="D53" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E53">
+        <v>6</v>
+      </c>
+      <c r="F53">
+        <v>2</v>
+      </c>
+      <c r="G53">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>52</v>
       </c>
@@ -3012,8 +3498,17 @@
       <c r="D54" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E54">
+        <v>6</v>
+      </c>
+      <c r="F54">
+        <v>2</v>
+      </c>
+      <c r="G54">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>53</v>
       </c>
@@ -3026,8 +3521,17 @@
       <c r="D55" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E55">
+        <v>6</v>
+      </c>
+      <c r="F55">
+        <v>2</v>
+      </c>
+      <c r="G55">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>54</v>
       </c>
@@ -3040,8 +3544,17 @@
       <c r="D56" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E56">
+        <v>6</v>
+      </c>
+      <c r="F56">
+        <v>2</v>
+      </c>
+      <c r="G56">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>55</v>
       </c>
@@ -3054,8 +3567,17 @@
       <c r="D57" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E57">
+        <v>6</v>
+      </c>
+      <c r="F57">
+        <v>2</v>
+      </c>
+      <c r="G57">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>56</v>
       </c>
@@ -3068,8 +3590,17 @@
       <c r="D58" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E58">
+        <v>6</v>
+      </c>
+      <c r="F58">
+        <v>2</v>
+      </c>
+      <c r="G58">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>57</v>
       </c>
@@ -3082,8 +3613,17 @@
       <c r="D59" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E59">
+        <v>6</v>
+      </c>
+      <c r="F59">
+        <v>2</v>
+      </c>
+      <c r="G59">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>58</v>
       </c>
@@ -3096,8 +3636,17 @@
       <c r="D60" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E60">
+        <v>6</v>
+      </c>
+      <c r="F60">
+        <v>2</v>
+      </c>
+      <c r="G60">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>59</v>
       </c>
@@ -3110,8 +3659,17 @@
       <c r="D61" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E61">
+        <v>6</v>
+      </c>
+      <c r="F61">
+        <v>2</v>
+      </c>
+      <c r="G61">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>60</v>
       </c>
@@ -3124,8 +3682,17 @@
       <c r="D62" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E62">
+        <v>7</v>
+      </c>
+      <c r="F62">
+        <v>2</v>
+      </c>
+      <c r="G62">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>61</v>
       </c>
@@ -3138,8 +3705,17 @@
       <c r="D63" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E63">
+        <v>7</v>
+      </c>
+      <c r="F63">
+        <v>2</v>
+      </c>
+      <c r="G63">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>62</v>
       </c>
@@ -3152,8 +3728,17 @@
       <c r="D64" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E64">
+        <v>7</v>
+      </c>
+      <c r="F64">
+        <v>2</v>
+      </c>
+      <c r="G64">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>63</v>
       </c>
@@ -3166,8 +3751,17 @@
       <c r="D65" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E65">
+        <v>7</v>
+      </c>
+      <c r="F65">
+        <v>2</v>
+      </c>
+      <c r="G65">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>64</v>
       </c>
@@ -3180,8 +3774,17 @@
       <c r="D66" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E66">
+        <v>7</v>
+      </c>
+      <c r="F66">
+        <v>2</v>
+      </c>
+      <c r="G66">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>65</v>
       </c>
@@ -3194,8 +3797,17 @@
       <c r="D67" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E67">
+        <v>7</v>
+      </c>
+      <c r="F67">
+        <v>2</v>
+      </c>
+      <c r="G67">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>66</v>
       </c>
@@ -3208,8 +3820,17 @@
       <c r="D68" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E68">
+        <v>7</v>
+      </c>
+      <c r="F68">
+        <v>2</v>
+      </c>
+      <c r="G68">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>67</v>
       </c>
@@ -3222,8 +3843,17 @@
       <c r="D69" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E69">
+        <v>7</v>
+      </c>
+      <c r="F69">
+        <v>2</v>
+      </c>
+      <c r="G69">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>68</v>
       </c>
@@ -3236,8 +3866,17 @@
       <c r="D70" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E70">
+        <v>7</v>
+      </c>
+      <c r="F70">
+        <v>2</v>
+      </c>
+      <c r="G70">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>69</v>
       </c>
@@ -3250,8 +3889,17 @@
       <c r="D71" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E71">
+        <v>7</v>
+      </c>
+      <c r="F71">
+        <v>2</v>
+      </c>
+      <c r="G71">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>70</v>
       </c>
@@ -3264,8 +3912,17 @@
       <c r="D72" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E72">
+        <v>8</v>
+      </c>
+      <c r="F72">
+        <v>2</v>
+      </c>
+      <c r="G72">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>71</v>
       </c>
@@ -3278,8 +3935,17 @@
       <c r="D73" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E73">
+        <v>8</v>
+      </c>
+      <c r="F73">
+        <v>2</v>
+      </c>
+      <c r="G73">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>72</v>
       </c>
@@ -3292,8 +3958,17 @@
       <c r="D74" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E74">
+        <v>8</v>
+      </c>
+      <c r="F74">
+        <v>2</v>
+      </c>
+      <c r="G74">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>73</v>
       </c>
@@ -3306,8 +3981,17 @@
       <c r="D75" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E75">
+        <v>8</v>
+      </c>
+      <c r="F75">
+        <v>2</v>
+      </c>
+      <c r="G75">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>74</v>
       </c>
@@ -3320,8 +4004,17 @@
       <c r="D76" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E76">
+        <v>8</v>
+      </c>
+      <c r="F76">
+        <v>2</v>
+      </c>
+      <c r="G76">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>75</v>
       </c>
@@ -3334,8 +4027,17 @@
       <c r="D77" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E77">
+        <v>8</v>
+      </c>
+      <c r="F77">
+        <v>3</v>
+      </c>
+      <c r="G77">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>76</v>
       </c>
@@ -3348,8 +4050,17 @@
       <c r="D78" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E78">
+        <v>8</v>
+      </c>
+      <c r="F78">
+        <v>3</v>
+      </c>
+      <c r="G78">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>77</v>
       </c>
@@ -3362,8 +4073,17 @@
       <c r="D79" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E79">
+        <v>8</v>
+      </c>
+      <c r="F79">
+        <v>3</v>
+      </c>
+      <c r="G79">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>78</v>
       </c>
@@ -3376,8 +4096,17 @@
       <c r="D80" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E80">
+        <v>8</v>
+      </c>
+      <c r="F80">
+        <v>3</v>
+      </c>
+      <c r="G80">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>79</v>
       </c>
@@ -3390,8 +4119,17 @@
       <c r="D81" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E81">
+        <v>8</v>
+      </c>
+      <c r="F81">
+        <v>3</v>
+      </c>
+      <c r="G81">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>80</v>
       </c>
@@ -3404,8 +4142,17 @@
       <c r="D82" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E82">
+        <v>9</v>
+      </c>
+      <c r="F82">
+        <v>3</v>
+      </c>
+      <c r="G82">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>81</v>
       </c>
@@ -3418,8 +4165,17 @@
       <c r="D83" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E83">
+        <v>9</v>
+      </c>
+      <c r="F83">
+        <v>3</v>
+      </c>
+      <c r="G83">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>82</v>
       </c>
@@ -3432,8 +4188,17 @@
       <c r="D84" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E84">
+        <v>9</v>
+      </c>
+      <c r="F84">
+        <v>3</v>
+      </c>
+      <c r="G84">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>83</v>
       </c>
@@ -3446,8 +4211,17 @@
       <c r="D85" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E85">
+        <v>9</v>
+      </c>
+      <c r="F85">
+        <v>3</v>
+      </c>
+      <c r="G85">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>84</v>
       </c>
@@ -3460,8 +4234,17 @@
       <c r="D86" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E86">
+        <v>9</v>
+      </c>
+      <c r="F86">
+        <v>3</v>
+      </c>
+      <c r="G86">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>85</v>
       </c>
@@ -3474,8 +4257,17 @@
       <c r="D87" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E87">
+        <v>9</v>
+      </c>
+      <c r="F87">
+        <v>3</v>
+      </c>
+      <c r="G87">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>86</v>
       </c>
@@ -3488,8 +4280,17 @@
       <c r="D88" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E88">
+        <v>9</v>
+      </c>
+      <c r="F88">
+        <v>3</v>
+      </c>
+      <c r="G88">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>87</v>
       </c>
@@ -3502,8 +4303,17 @@
       <c r="D89" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E89">
+        <v>9</v>
+      </c>
+      <c r="F89">
+        <v>3</v>
+      </c>
+      <c r="G89">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>88</v>
       </c>
@@ -3516,8 +4326,17 @@
       <c r="D90" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E90">
+        <v>9</v>
+      </c>
+      <c r="F90">
+        <v>3</v>
+      </c>
+      <c r="G90">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>89</v>
       </c>
@@ -3530,8 +4349,17 @@
       <c r="D91" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E91">
+        <v>9</v>
+      </c>
+      <c r="F91">
+        <v>3</v>
+      </c>
+      <c r="G91">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>90</v>
       </c>
@@ -3544,8 +4372,17 @@
       <c r="D92" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E92">
+        <v>9</v>
+      </c>
+      <c r="F92">
+        <v>3</v>
+      </c>
+      <c r="G92">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>91</v>
       </c>
@@ -3558,8 +4395,17 @@
       <c r="D93" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E93">
+        <v>9</v>
+      </c>
+      <c r="F93">
+        <v>3</v>
+      </c>
+      <c r="G93">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>92</v>
       </c>
@@ -3572,8 +4418,17 @@
       <c r="D94" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E94">
+        <v>9</v>
+      </c>
+      <c r="F94">
+        <v>3</v>
+      </c>
+      <c r="G94">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>93</v>
       </c>
@@ -3586,8 +4441,17 @@
       <c r="D95" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E95">
+        <v>9</v>
+      </c>
+      <c r="F95">
+        <v>3</v>
+      </c>
+      <c r="G95">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>94</v>
       </c>
@@ -3600,8 +4464,17 @@
       <c r="D96" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E96">
+        <v>9</v>
+      </c>
+      <c r="F96">
+        <v>3</v>
+      </c>
+      <c r="G96">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>95</v>
       </c>
@@ -3614,8 +4487,17 @@
       <c r="D97" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E97">
+        <v>9</v>
+      </c>
+      <c r="F97">
+        <v>3</v>
+      </c>
+      <c r="G97">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>96</v>
       </c>
@@ -3628,8 +4510,17 @@
       <c r="D98" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E98">
+        <v>9</v>
+      </c>
+      <c r="F98">
+        <v>3</v>
+      </c>
+      <c r="G98">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>97</v>
       </c>
@@ -3642,8 +4533,17 @@
       <c r="D99" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E99">
+        <v>9</v>
+      </c>
+      <c r="F99">
+        <v>3</v>
+      </c>
+      <c r="G99">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>98</v>
       </c>
@@ -3656,8 +4556,17 @@
       <c r="D100" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E100">
+        <v>9</v>
+      </c>
+      <c r="F100">
+        <v>3</v>
+      </c>
+      <c r="G100">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>99</v>
       </c>
@@ -3670,8 +4579,17 @@
       <c r="D101" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E101">
+        <v>9</v>
+      </c>
+      <c r="F101">
+        <v>3</v>
+      </c>
+      <c r="G101">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>100</v>
       </c>
@@ -3684,8 +4602,17 @@
       <c r="D102" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E102">
+        <v>9</v>
+      </c>
+      <c r="F102">
+        <v>3</v>
+      </c>
+      <c r="G102">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>101</v>
       </c>
@@ -3698,8 +4625,17 @@
       <c r="D103" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E103">
+        <v>9</v>
+      </c>
+      <c r="F103">
+        <v>3</v>
+      </c>
+      <c r="G103">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>102</v>
       </c>
@@ -3712,8 +4648,17 @@
       <c r="D104" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E104">
+        <v>9</v>
+      </c>
+      <c r="F104">
+        <v>3</v>
+      </c>
+      <c r="G104">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>103</v>
       </c>
@@ -3726,8 +4671,17 @@
       <c r="D105" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E105">
+        <v>9</v>
+      </c>
+      <c r="F105">
+        <v>3</v>
+      </c>
+      <c r="G105">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>104</v>
       </c>
@@ -3740,8 +4694,17 @@
       <c r="D106" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E106">
+        <v>9</v>
+      </c>
+      <c r="F106">
+        <v>3</v>
+      </c>
+      <c r="G106">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>105</v>
       </c>
@@ -3754,8 +4717,17 @@
       <c r="D107" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E107">
+        <v>9</v>
+      </c>
+      <c r="F107">
+        <v>3</v>
+      </c>
+      <c r="G107">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>106</v>
       </c>
@@ -3768,8 +4740,17 @@
       <c r="D108" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E108">
+        <v>9</v>
+      </c>
+      <c r="F108">
+        <v>3</v>
+      </c>
+      <c r="G108">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>107</v>
       </c>
@@ -3782,8 +4763,17 @@
       <c r="D109" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E109">
+        <v>9</v>
+      </c>
+      <c r="F109">
+        <v>3</v>
+      </c>
+      <c r="G109">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>108</v>
       </c>
@@ -3796,8 +4786,17 @@
       <c r="D110" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E110">
+        <v>9</v>
+      </c>
+      <c r="F110">
+        <v>3</v>
+      </c>
+      <c r="G110">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>109</v>
       </c>
@@ -3810,8 +4809,17 @@
       <c r="D111" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E111">
+        <v>9</v>
+      </c>
+      <c r="F111">
+        <v>3</v>
+      </c>
+      <c r="G111">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>110</v>
       </c>
@@ -3824,8 +4832,17 @@
       <c r="D112" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E112">
+        <v>9</v>
+      </c>
+      <c r="F112">
+        <v>3</v>
+      </c>
+      <c r="G112">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>111</v>
       </c>
@@ -3838,8 +4855,17 @@
       <c r="D113" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E113">
+        <v>9</v>
+      </c>
+      <c r="F113">
+        <v>3</v>
+      </c>
+      <c r="G113">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>112</v>
       </c>
@@ -3852,8 +4878,17 @@
       <c r="D114" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E114">
+        <v>9</v>
+      </c>
+      <c r="F114">
+        <v>3</v>
+      </c>
+      <c r="G114">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>113</v>
       </c>
@@ -3866,8 +4901,17 @@
       <c r="D115" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E115">
+        <v>9</v>
+      </c>
+      <c r="F115">
+        <v>3</v>
+      </c>
+      <c r="G115">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>114</v>
       </c>
@@ -3880,8 +4924,17 @@
       <c r="D116" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E116">
+        <v>9</v>
+      </c>
+      <c r="F116">
+        <v>3</v>
+      </c>
+      <c r="G116">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>115</v>
       </c>
@@ -3894,8 +4947,17 @@
       <c r="D117" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E117">
+        <v>9</v>
+      </c>
+      <c r="F117">
+        <v>3</v>
+      </c>
+      <c r="G117">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>116</v>
       </c>
@@ -3908,8 +4970,17 @@
       <c r="D118" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E118">
+        <v>9</v>
+      </c>
+      <c r="F118">
+        <v>3</v>
+      </c>
+      <c r="G118">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>117</v>
       </c>
@@ -3922,8 +4993,17 @@
       <c r="D119" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E119">
+        <v>9</v>
+      </c>
+      <c r="F119">
+        <v>3</v>
+      </c>
+      <c r="G119">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>118</v>
       </c>
@@ -3936,8 +5016,17 @@
       <c r="D120" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E120">
+        <v>9</v>
+      </c>
+      <c r="F120">
+        <v>3</v>
+      </c>
+      <c r="G120">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>119</v>
       </c>
@@ -3950,8 +5039,17 @@
       <c r="D121" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E121">
+        <v>9</v>
+      </c>
+      <c r="F121">
+        <v>3</v>
+      </c>
+      <c r="G121">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>120</v>
       </c>
@@ -3963,6 +5061,15 @@
       </c>
       <c r="D122" s="4" t="s">
         <v>168</v>
+      </c>
+      <c r="E122">
+        <v>9</v>
+      </c>
+      <c r="F122">
+        <v>3</v>
+      </c>
+      <c r="G122">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed fitting scheme for LOS clinical assessment version
</commit_message>
<xml_diff>
--- a/lsh_data_processing/lsh_coding.xlsx
+++ b/lsh_data_processing/lsh_coding.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10307"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rjs/projects/covid/BCS/lsh_data_processing/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/solviro/Documents/COVID-19/BCS/lsh_data_processing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3091E55-57DF-F94D-A332-B53C3306A2A3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F34DECB9-271F-8B4E-9B2F-71C54D5E409B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4740" yWindow="-20380" windowWidth="25040" windowHeight="14000" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20900" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="lsh_covid_groups" sheetId="3" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="176">
   <si>
     <t>text_out_category_raw</t>
   </si>
@@ -308,9 +308,6 @@
     <t>clinical_assessment_category_all</t>
   </si>
   <si>
-    <t>clinical_assessment_category_simple</t>
-  </si>
-  <si>
     <t>Blár</t>
   </si>
   <si>
@@ -479,9 +476,6 @@
     <t>Dagdeild</t>
   </si>
   <si>
-    <t>clinical_assessment_category_order_simple</t>
-  </si>
-  <si>
     <t>clinical_assessment_category_order_all</t>
   </si>
   <si>
@@ -555,6 +549,18 @@
   </si>
   <si>
     <t>age_group_order_simple</t>
+  </si>
+  <si>
+    <t>clinical_assessment_category_simple_red</t>
+  </si>
+  <si>
+    <t>clinical_assessment_category_simple_green</t>
+  </si>
+  <si>
+    <t>clinical_assessment_category_order_simple_red</t>
+  </si>
+  <si>
+    <t>clinical_assessment_category_order_simple_green</t>
   </si>
 </sst>
 </file>
@@ -1500,7 +1506,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B21" t="s">
         <v>31</v>
@@ -1517,13 +1523,13 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B22" t="s">
         <v>12</v>
       </c>
       <c r="C22" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D22" t="s">
         <v>10</v>
@@ -1534,7 +1540,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B23" t="s">
         <v>29</v>
@@ -1551,7 +1557,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B24" t="s">
         <v>31</v>
@@ -1568,10 +1574,10 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>145</v>
+      </c>
+      <c r="B25" t="s">
         <v>146</v>
-      </c>
-      <c r="B25" t="s">
-        <v>147</v>
       </c>
       <c r="C25" t="s">
         <v>35</v>
@@ -1585,7 +1591,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B26" t="s">
         <v>29</v>
@@ -1602,7 +1608,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B27" t="s">
         <v>29</v>
@@ -1780,21 +1786,24 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="28.33203125" customWidth="1"/>
-    <col min="2" max="2" width="30.83203125" customWidth="1"/>
-    <col min="3" max="3" width="32.33203125" customWidth="1"/>
-    <col min="4" max="4" width="33" customWidth="1"/>
+    <col min="2" max="2" width="26.5" customWidth="1"/>
+    <col min="3" max="3" width="33.5" customWidth="1"/>
+    <col min="4" max="4" width="35.83203125" customWidth="1"/>
+    <col min="5" max="5" width="37.5" customWidth="1"/>
+    <col min="6" max="6" width="39.5" customWidth="1"/>
+    <col min="7" max="7" width="32.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>89</v>
       </c>
@@ -1802,131 +1811,179 @@
         <v>90</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>91</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>92</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>98</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C4" t="s">
+        <v>99</v>
+      </c>
+      <c r="D4" t="s">
+        <v>99</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>103</v>
       </c>
-      <c r="D2">
-        <v>2</v>
-      </c>
-      <c r="E2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="B5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D5" t="s">
         <v>99</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>94</v>
+      </c>
+      <c r="B6" t="s">
         <v>100</v>
       </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>94</v>
-      </c>
-      <c r="B4" t="s">
-        <v>100</v>
-      </c>
-      <c r="C4" t="s">
-        <v>100</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>104</v>
-      </c>
-      <c r="B5" t="s">
-        <v>105</v>
-      </c>
-      <c r="C5" t="s">
-        <v>103</v>
-      </c>
-      <c r="D5">
-        <v>2</v>
-      </c>
-      <c r="E5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>95</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>101</v>
       </c>
-      <c r="C6" t="s">
-        <v>102</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
+      <c r="D6" t="s">
+        <v>101</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C7" t="s">
-        <v>102</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
+        <v>101</v>
+      </c>
+      <c r="D7" t="s">
+        <v>101</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C8" t="s">
-        <v>103</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
+        <v>102</v>
+      </c>
+      <c r="D8" t="s">
+        <v>102</v>
       </c>
       <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="G8">
         <v>4</v>
       </c>
     </row>
@@ -2011,22 +2068,22 @@
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -2051,27 +2108,27 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B1" t="s">
         <v>111</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>113</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B2" t="s">
         <v>115</v>
       </c>
-      <c r="B2" t="s">
-        <v>116</v>
-      </c>
       <c r="C2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -2079,13 +2136,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B3" t="s">
         <v>117</v>
       </c>
-      <c r="B3" t="s">
-        <v>118</v>
-      </c>
       <c r="C3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -2093,13 +2150,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B4" t="s">
         <v>119</v>
       </c>
-      <c r="B4" t="s">
-        <v>120</v>
-      </c>
       <c r="C4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D4">
         <v>3</v>
@@ -2127,21 +2184,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B1" t="s">
         <v>121</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>122</v>
-      </c>
-      <c r="C1" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B2" t="s">
         <v>124</v>
-      </c>
-      <c r="B2" t="s">
-        <v>125</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -2149,10 +2206,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B3" t="s">
         <v>126</v>
-      </c>
-      <c r="B3" t="s">
-        <v>127</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -2160,10 +2217,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B4" t="s">
         <v>128</v>
-      </c>
-      <c r="B4" t="s">
-        <v>129</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -2171,10 +2228,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>129</v>
+      </c>
+      <c r="B5" t="s">
         <v>130</v>
-      </c>
-      <c r="B5" t="s">
-        <v>131</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -2182,10 +2239,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>131</v>
+      </c>
+      <c r="B6" t="s">
         <v>132</v>
-      </c>
-      <c r="B6" t="s">
-        <v>133</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -2193,10 +2250,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>133</v>
+      </c>
+      <c r="B7" t="s">
         <v>134</v>
-      </c>
-      <c r="B7" t="s">
-        <v>135</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -2204,10 +2261,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>135</v>
+      </c>
+      <c r="B8" t="s">
         <v>136</v>
-      </c>
-      <c r="B8" t="s">
-        <v>137</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -2215,10 +2272,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>137</v>
+      </c>
+      <c r="B9" t="s">
         <v>138</v>
-      </c>
-      <c r="B9" t="s">
-        <v>139</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -2226,10 +2283,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>139</v>
+      </c>
+      <c r="B10" t="s">
         <v>140</v>
-      </c>
-      <c r="B10" t="s">
-        <v>141</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -2237,10 +2294,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>141</v>
+      </c>
+      <c r="B11" t="s">
         <v>142</v>
-      </c>
-      <c r="B11" t="s">
-        <v>143</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -2255,7 +2312,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F50DD301-9CCE-6744-864C-185ECBAFA9CA}">
   <dimension ref="A1:G122"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
+    <sheetView zoomScale="99" workbookViewId="0">
       <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
@@ -2268,25 +2325,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C1" t="s">
         <v>152</v>
       </c>
-      <c r="B1" t="s">
-        <v>164</v>
-      </c>
-      <c r="C1" t="s">
-        <v>154</v>
-      </c>
       <c r="D1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E1" t="s">
+        <v>169</v>
+      </c>
+      <c r="F1" t="s">
+        <v>170</v>
+      </c>
+      <c r="G1" t="s">
         <v>171</v>
-      </c>
-      <c r="F1" t="s">
-        <v>172</v>
-      </c>
-      <c r="G1" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -2294,13 +2351,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -2317,13 +2374,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -2340,13 +2397,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -2363,13 +2420,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -2386,13 +2443,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -2409,13 +2466,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -2432,13 +2489,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -2455,13 +2512,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -2478,13 +2535,13 @@
         <v>8</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -2501,13 +2558,13 @@
         <v>9</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E11">
         <v>1</v>
@@ -2524,13 +2581,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E12">
         <v>2</v>
@@ -2547,13 +2604,13 @@
         <v>11</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E13">
         <v>2</v>
@@ -2570,13 +2627,13 @@
         <v>12</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E14">
         <v>2</v>
@@ -2593,13 +2650,13 @@
         <v>13</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E15">
         <v>2</v>
@@ -2616,13 +2673,13 @@
         <v>14</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E16">
         <v>2</v>
@@ -2639,13 +2696,13 @@
         <v>15</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E17">
         <v>2</v>
@@ -2662,13 +2719,13 @@
         <v>16</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E18">
         <v>2</v>
@@ -2685,13 +2742,13 @@
         <v>17</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E19">
         <v>2</v>
@@ -2708,13 +2765,13 @@
         <v>18</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E20">
         <v>2</v>
@@ -2731,13 +2788,13 @@
         <v>19</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E21">
         <v>2</v>
@@ -2754,13 +2811,13 @@
         <v>20</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E22">
         <v>3</v>
@@ -2777,13 +2834,13 @@
         <v>21</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E23">
         <v>3</v>
@@ -2800,13 +2857,13 @@
         <v>22</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E24">
         <v>3</v>
@@ -2823,13 +2880,13 @@
         <v>23</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E25">
         <v>3</v>
@@ -2846,13 +2903,13 @@
         <v>24</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E26">
         <v>3</v>
@@ -2869,13 +2926,13 @@
         <v>25</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E27">
         <v>3</v>
@@ -2892,13 +2949,13 @@
         <v>26</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E28">
         <v>3</v>
@@ -2915,13 +2972,13 @@
         <v>27</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E29">
         <v>3</v>
@@ -2938,13 +2995,13 @@
         <v>28</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E30">
         <v>3</v>
@@ -2961,13 +3018,13 @@
         <v>29</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E31">
         <v>3</v>
@@ -2984,13 +3041,13 @@
         <v>30</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E32">
         <v>4</v>
@@ -3007,13 +3064,13 @@
         <v>31</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E33">
         <v>4</v>
@@ -3030,13 +3087,13 @@
         <v>32</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E34">
         <v>4</v>
@@ -3053,13 +3110,13 @@
         <v>33</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E35">
         <v>4</v>
@@ -3076,13 +3133,13 @@
         <v>34</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E36">
         <v>4</v>
@@ -3099,13 +3156,13 @@
         <v>35</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E37">
         <v>4</v>
@@ -3122,13 +3179,13 @@
         <v>36</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E38">
         <v>4</v>
@@ -3145,13 +3202,13 @@
         <v>37</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E39">
         <v>4</v>
@@ -3168,13 +3225,13 @@
         <v>38</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E40">
         <v>4</v>
@@ -3191,13 +3248,13 @@
         <v>39</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E41">
         <v>4</v>
@@ -3214,13 +3271,13 @@
         <v>40</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E42">
         <v>5</v>
@@ -3237,13 +3294,13 @@
         <v>41</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E43">
         <v>5</v>
@@ -3260,13 +3317,13 @@
         <v>42</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E44">
         <v>5</v>
@@ -3283,13 +3340,13 @@
         <v>43</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E45">
         <v>5</v>
@@ -3306,13 +3363,13 @@
         <v>44</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E46">
         <v>5</v>
@@ -3329,13 +3386,13 @@
         <v>45</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E47">
         <v>5</v>
@@ -3352,13 +3409,13 @@
         <v>46</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E48">
         <v>5</v>
@@ -3375,13 +3432,13 @@
         <v>47</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E49">
         <v>5</v>
@@ -3398,13 +3455,13 @@
         <v>48</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E50">
         <v>5</v>
@@ -3421,13 +3478,13 @@
         <v>49</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E51">
         <v>5</v>
@@ -3444,13 +3501,13 @@
         <v>50</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E52">
         <v>6</v>
@@ -3467,13 +3524,13 @@
         <v>51</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E53">
         <v>6</v>
@@ -3490,13 +3547,13 @@
         <v>52</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E54">
         <v>6</v>
@@ -3513,13 +3570,13 @@
         <v>53</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E55">
         <v>6</v>
@@ -3536,13 +3593,13 @@
         <v>54</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E56">
         <v>6</v>
@@ -3559,13 +3616,13 @@
         <v>55</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E57">
         <v>6</v>
@@ -3582,13 +3639,13 @@
         <v>56</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E58">
         <v>6</v>
@@ -3605,13 +3662,13 @@
         <v>57</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E59">
         <v>6</v>
@@ -3628,13 +3685,13 @@
         <v>58</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E60">
         <v>6</v>
@@ -3651,13 +3708,13 @@
         <v>59</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E61">
         <v>6</v>
@@ -3674,13 +3731,13 @@
         <v>60</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E62">
         <v>7</v>
@@ -3697,13 +3754,13 @@
         <v>61</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E63">
         <v>7</v>
@@ -3720,13 +3777,13 @@
         <v>62</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E64">
         <v>7</v>
@@ -3743,13 +3800,13 @@
         <v>63</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E65">
         <v>7</v>
@@ -3766,13 +3823,13 @@
         <v>64</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E66">
         <v>7</v>
@@ -3789,13 +3846,13 @@
         <v>65</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E67">
         <v>7</v>
@@ -3812,13 +3869,13 @@
         <v>66</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E68">
         <v>7</v>
@@ -3835,13 +3892,13 @@
         <v>67</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E69">
         <v>7</v>
@@ -3858,13 +3915,13 @@
         <v>68</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E70">
         <v>7</v>
@@ -3881,13 +3938,13 @@
         <v>69</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E71">
         <v>7</v>
@@ -3904,13 +3961,13 @@
         <v>70</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E72">
         <v>8</v>
@@ -3927,13 +3984,13 @@
         <v>71</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E73">
         <v>8</v>
@@ -3950,13 +4007,13 @@
         <v>72</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D74" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E74">
         <v>8</v>
@@ -3973,13 +4030,13 @@
         <v>73</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E75">
         <v>8</v>
@@ -3996,13 +4053,13 @@
         <v>74</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E76">
         <v>8</v>
@@ -4019,13 +4076,13 @@
         <v>75</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E77">
         <v>8</v>
@@ -4042,13 +4099,13 @@
         <v>76</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D78" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E78">
         <v>8</v>
@@ -4065,13 +4122,13 @@
         <v>77</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D79" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E79">
         <v>8</v>
@@ -4088,13 +4145,13 @@
         <v>78</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D80" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E80">
         <v>8</v>
@@ -4111,13 +4168,13 @@
         <v>79</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D81" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E81">
         <v>8</v>
@@ -4134,13 +4191,13 @@
         <v>80</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D82" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E82">
         <v>9</v>
@@ -4157,13 +4214,13 @@
         <v>81</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D83" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E83">
         <v>9</v>
@@ -4180,13 +4237,13 @@
         <v>82</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D84" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E84">
         <v>9</v>
@@ -4203,13 +4260,13 @@
         <v>83</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D85" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E85">
         <v>9</v>
@@ -4226,13 +4283,13 @@
         <v>84</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D86" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E86">
         <v>9</v>
@@ -4249,13 +4306,13 @@
         <v>85</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D87" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E87">
         <v>9</v>
@@ -4272,13 +4329,13 @@
         <v>86</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D88" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E88">
         <v>9</v>
@@ -4295,13 +4352,13 @@
         <v>87</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D89" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E89">
         <v>9</v>
@@ -4318,13 +4375,13 @@
         <v>88</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D90" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E90">
         <v>9</v>
@@ -4341,13 +4398,13 @@
         <v>89</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D91" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E91">
         <v>9</v>
@@ -4364,13 +4421,13 @@
         <v>90</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D92" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E92">
         <v>9</v>
@@ -4387,13 +4444,13 @@
         <v>91</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D93" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E93">
         <v>9</v>
@@ -4410,13 +4467,13 @@
         <v>92</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D94" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E94">
         <v>9</v>
@@ -4433,13 +4490,13 @@
         <v>93</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D95" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E95">
         <v>9</v>
@@ -4456,13 +4513,13 @@
         <v>94</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C96" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D96" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E96">
         <v>9</v>
@@ -4479,13 +4536,13 @@
         <v>95</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D97" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E97">
         <v>9</v>
@@ -4502,13 +4559,13 @@
         <v>96</v>
       </c>
       <c r="B98" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D98" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E98">
         <v>9</v>
@@ -4525,13 +4582,13 @@
         <v>97</v>
       </c>
       <c r="B99" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D99" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E99">
         <v>9</v>
@@ -4548,13 +4605,13 @@
         <v>98</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D100" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E100">
         <v>9</v>
@@ -4571,13 +4628,13 @@
         <v>99</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D101" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E101">
         <v>9</v>
@@ -4594,13 +4651,13 @@
         <v>100</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D102" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E102">
         <v>9</v>
@@ -4617,13 +4674,13 @@
         <v>101</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D103" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E103">
         <v>9</v>
@@ -4640,13 +4697,13 @@
         <v>102</v>
       </c>
       <c r="B104" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D104" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E104">
         <v>9</v>
@@ -4663,13 +4720,13 @@
         <v>103</v>
       </c>
       <c r="B105" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D105" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E105">
         <v>9</v>
@@ -4686,13 +4743,13 @@
         <v>104</v>
       </c>
       <c r="B106" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D106" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E106">
         <v>9</v>
@@ -4709,13 +4766,13 @@
         <v>105</v>
       </c>
       <c r="B107" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D107" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E107">
         <v>9</v>
@@ -4732,13 +4789,13 @@
         <v>106</v>
       </c>
       <c r="B108" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D108" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E108">
         <v>9</v>
@@ -4755,13 +4812,13 @@
         <v>107</v>
       </c>
       <c r="B109" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C109" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D109" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E109">
         <v>9</v>
@@ -4778,13 +4835,13 @@
         <v>108</v>
       </c>
       <c r="B110" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D110" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E110">
         <v>9</v>
@@ -4801,13 +4858,13 @@
         <v>109</v>
       </c>
       <c r="B111" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D111" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E111">
         <v>9</v>
@@ -4824,13 +4881,13 @@
         <v>110</v>
       </c>
       <c r="B112" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C112" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D112" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E112">
         <v>9</v>
@@ -4847,13 +4904,13 @@
         <v>111</v>
       </c>
       <c r="B113" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D113" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E113">
         <v>9</v>
@@ -4870,13 +4927,13 @@
         <v>112</v>
       </c>
       <c r="B114" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D114" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E114">
         <v>9</v>
@@ -4893,13 +4950,13 @@
         <v>113</v>
       </c>
       <c r="B115" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C115" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D115" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E115">
         <v>9</v>
@@ -4916,13 +4973,13 @@
         <v>114</v>
       </c>
       <c r="B116" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D116" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E116">
         <v>9</v>
@@ -4939,13 +4996,13 @@
         <v>115</v>
       </c>
       <c r="B117" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C117" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D117" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E117">
         <v>9</v>
@@ -4962,13 +5019,13 @@
         <v>116</v>
       </c>
       <c r="B118" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C118" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D118" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E118">
         <v>9</v>
@@ -4985,13 +5042,13 @@
         <v>117</v>
       </c>
       <c r="B119" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C119" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D119" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E119">
         <v>9</v>
@@ -5008,13 +5065,13 @@
         <v>118</v>
       </c>
       <c r="B120" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C120" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D120" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E120">
         <v>9</v>
@@ -5031,13 +5088,13 @@
         <v>119</v>
       </c>
       <c r="B121" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C121" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D121" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E121">
         <v>9</v>
@@ -5054,13 +5111,13 @@
         <v>120</v>
       </c>
       <c r="B122" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C122" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D122" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E122">
         <v>9</v>

</xml_diff>

<commit_message>
Added new text out category
</commit_message>
<xml_diff>
--- a/lsh_data_processing/lsh_coding.xlsx
+++ b/lsh_data_processing/lsh_coding.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10307"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/solviro/Documents/COVID-19/BCS/lsh_data_processing/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rjs/projects/covid/BCS/lsh_data_processing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F34DECB9-271F-8B4E-9B2F-71C54D5E409B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{634FE275-BA1D-164F-9731-C33C26FEB3B2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20900" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14540" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="lsh_covid_groups" sheetId="3" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="177">
   <si>
     <t>text_out_category_raw</t>
   </si>
@@ -561,6 +561,9 @@
   </si>
   <si>
     <t>clinical_assessment_category_order_simple_green</t>
+  </si>
+  <si>
+    <t>Dvalarheimili</t>
   </si>
 </sst>
 </file>
@@ -1635,10 +1638,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" zoomScale="141" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1772,6 +1775,20 @@
       </c>
       <c r="D9" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>176</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1788,7 +1805,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added new unit categores and fixed bug.
</commit_message>
<xml_diff>
--- a/lsh_data_processing/lsh_coding.xlsx
+++ b/lsh_data_processing/lsh_coding.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10307"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rjs/projects/covid/BCS/lsh_data_processing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{634FE275-BA1D-164F-9731-C33C26FEB3B2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF682697-8047-8648-8A9A-EADC3E535F07}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14540" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14460" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="lsh_covid_groups" sheetId="3" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="181">
   <si>
     <t>text_out_category_raw</t>
   </si>
@@ -564,6 +564,18 @@
   </si>
   <si>
     <t>Dvalarheimili</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bráðaöldrunarlækningadeild (Fv-B4)                                                                                           </t>
+  </si>
+  <si>
+    <t>Fv-A3 GD Svefnrannsókna</t>
+  </si>
+  <si>
+    <t>Hb-21B GD Fósturgreiningadeild</t>
+  </si>
+  <si>
+    <t>Hb-31E GD Geðsviðs</t>
   </si>
 </sst>
 </file>
@@ -1152,10 +1164,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView topLeftCell="B11" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1626,6 +1638,74 @@
         <v>1</v>
       </c>
     </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>177</v>
+      </c>
+      <c r="B28" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" t="s">
+        <v>33</v>
+      </c>
+      <c r="D28" t="s">
+        <v>10</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>178</v>
+      </c>
+      <c r="B29" t="s">
+        <v>31</v>
+      </c>
+      <c r="C29" t="s">
+        <v>35</v>
+      </c>
+      <c r="D29" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>179</v>
+      </c>
+      <c r="B30" t="s">
+        <v>31</v>
+      </c>
+      <c r="C30" t="s">
+        <v>35</v>
+      </c>
+      <c r="D30" t="s">
+        <v>10</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>180</v>
+      </c>
+      <c r="B31" t="s">
+        <v>31</v>
+      </c>
+      <c r="C31" t="s">
+        <v>35</v>
+      </c>
+      <c r="D31" t="s">
+        <v>10</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1640,7 +1720,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="141" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView zoomScale="141" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added new unit category
</commit_message>
<xml_diff>
--- a/lsh_data_processing/lsh_coding.xlsx
+++ b/lsh_data_processing/lsh_coding.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rjs/projects/covid/BCS/lsh_data_processing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF682697-8047-8648-8A9A-EADC3E535F07}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DEAB84A-FE19-654D-A721-CDCDC39295D6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14460" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="lsh_covid_groups" sheetId="3" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="182">
   <si>
     <t>text_out_category_raw</t>
   </si>
@@ -576,6 +576,9 @@
   </si>
   <si>
     <t>Hb-31E GD Geðsviðs</t>
+  </si>
+  <si>
+    <t>Fv-G3 GD Bæklunarlækninga</t>
   </si>
 </sst>
 </file>
@@ -1164,10 +1167,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1703,6 +1706,23 @@
         <v>10</v>
       </c>
       <c r="E31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>181</v>
+      </c>
+      <c r="B32" t="s">
+        <v>31</v>
+      </c>
+      <c r="C32" t="s">
+        <v>35</v>
+      </c>
+      <c r="D32" t="s">
+        <v>10</v>
+      </c>
+      <c r="E32">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changed coding for Bráðalækningaöldrunardeild to fix bug in date of diagnosis for one patient. Added new outpatient clinic.
</commit_message>
<xml_diff>
--- a/lsh_data_processing/lsh_coding.xlsx
+++ b/lsh_data_processing/lsh_coding.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rjs/projects/covid/BCS/lsh_data_processing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DEAB84A-FE19-654D-A721-CDCDC39295D6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19437520-DFA4-514F-8E73-5BF6D79D7B37}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="183">
   <si>
     <t>text_out_category_raw</t>
   </si>
@@ -579,6 +579,9 @@
   </si>
   <si>
     <t>Fv-G3 GD Bæklunarlækninga</t>
+  </si>
+  <si>
+    <t>Ei37 GD Augnlækninga</t>
   </si>
 </sst>
 </file>
@@ -1167,10 +1170,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1646,16 +1649,16 @@
         <v>177</v>
       </c>
       <c r="B28" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C28" t="s">
-        <v>33</v>
+        <v>61</v>
       </c>
       <c r="D28" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="E28">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -1723,6 +1726,23 @@
         <v>10</v>
       </c>
       <c r="E32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>182</v>
+      </c>
+      <c r="B33" t="s">
+        <v>31</v>
+      </c>
+      <c r="C33" t="s">
+        <v>35</v>
+      </c>
+      <c r="D33" t="s">
+        <v>10</v>
+      </c>
+      <c r="E33">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
transition summary extended to take in time_splitting_variable
</commit_message>
<xml_diff>
--- a/lsh_data_processing/lsh_coding.xlsx
+++ b/lsh_data_processing/lsh_coding.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/solviro/Documents/COVID-19/BCS/lsh_data_processing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DC10D84-E5E6-964E-8DF9-930D4AD5DBC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B7795B1-AC91-7C49-A5ED-3940C38F223A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33420" yWindow="4020" windowWidth="25600" windowHeight="14540" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-35380" yWindow="460" windowWidth="25600" windowHeight="14540" firstSheet="3" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="lsh_covid_groups" sheetId="3" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="priority_categories" sheetId="7" r:id="rId7"/>
     <sheet name="comorbidities" sheetId="8" r:id="rId8"/>
     <sheet name="age_groups" sheetId="9" r:id="rId9"/>
+    <sheet name="length_of_stay_categories" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="140001"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="826" uniqueCount="207">
   <si>
     <t>text_out_category_raw</t>
   </si>
@@ -567,6 +568,93 @@
   </si>
   <si>
     <t>age_simple_order</t>
+  </si>
+  <si>
+    <t>Annað sjúkrahús</t>
+  </si>
+  <si>
+    <t>Flutningur á annað sjúkrahús</t>
+  </si>
+  <si>
+    <t>external_transfer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bráðaöldrunarlækningadeild (Fv-B4)                                                                                           </t>
+  </si>
+  <si>
+    <t>Fv-A3 GD Svefnrannsókna</t>
+  </si>
+  <si>
+    <t>Hb-21B GD Fósturgreiningadeild</t>
+  </si>
+  <si>
+    <t>Hb-31E GD Geðsviðs</t>
+  </si>
+  <si>
+    <t>Fv-G3 GD Bæklunarlækninga</t>
+  </si>
+  <si>
+    <t>Ei37 GD Augnlækninga</t>
+  </si>
+  <si>
+    <t>Hb-21AM GD Kvenna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hb-10D GD Hjartagátt                                                                                                                      </t>
+  </si>
+  <si>
+    <t>Hb-10E GD Melting, hjúkrun og lyfjagjafir</t>
+  </si>
+  <si>
+    <t>Hb-11A GD Þvagfæra</t>
+  </si>
+  <si>
+    <t>Hb-11C DD Krabbameins</t>
+  </si>
+  <si>
+    <t>Hb-21A DD Kvenlækningadeildar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hb-11C GD Krabbameins                                                                                        </t>
+  </si>
+  <si>
+    <t>Fv-E1 RD Hjartarannsóknastofa</t>
+  </si>
+  <si>
+    <t>Rannsókn</t>
+  </si>
+  <si>
+    <t>Fv-E2 GD Taugalækninga</t>
+  </si>
+  <si>
+    <t>Fv-E2 RD Taugarannsókn</t>
+  </si>
+  <si>
+    <t>length_of_stay</t>
+  </si>
+  <si>
+    <t>length_of_stay_simple</t>
+  </si>
+  <si>
+    <t>1-13</t>
+  </si>
+  <si>
+    <t>14+</t>
+  </si>
+  <si>
+    <t>length_of_stay_three</t>
+  </si>
+  <si>
+    <t>1-6</t>
+  </si>
+  <si>
+    <t>7-13</t>
+  </si>
+  <si>
+    <t>length_of_stay_simple_order</t>
+  </si>
+  <si>
+    <t>length_of_stay_three_order</t>
   </si>
 </sst>
 </file>
@@ -580,12 +668,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF333333"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
@@ -612,6 +694,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -657,28 +745,25 @@
   </borders>
   <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="13">
@@ -1095,6 +1180,1064 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85754964-25F9-724F-B597-4C81CCFECB89}">
+  <dimension ref="A1:E61"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.5" customWidth="1"/>
+    <col min="2" max="2" width="20.5" style="3" customWidth="1"/>
+    <col min="3" max="3" width="17.5" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D17">
+        <v>2</v>
+      </c>
+      <c r="E17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+      <c r="E18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
+      <c r="E19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D20">
+        <v>2</v>
+      </c>
+      <c r="E20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D21">
+        <v>2</v>
+      </c>
+      <c r="E21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D22">
+        <v>2</v>
+      </c>
+      <c r="E22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D23">
+        <v>2</v>
+      </c>
+      <c r="E23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D24">
+        <v>2</v>
+      </c>
+      <c r="E24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D25">
+        <v>2</v>
+      </c>
+      <c r="E25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D26">
+        <v>2</v>
+      </c>
+      <c r="E26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D27">
+        <v>2</v>
+      </c>
+      <c r="E27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D28">
+        <v>2</v>
+      </c>
+      <c r="E28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D29">
+        <v>2</v>
+      </c>
+      <c r="E29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D30">
+        <v>2</v>
+      </c>
+      <c r="E30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D31">
+        <v>2</v>
+      </c>
+      <c r="E31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D32">
+        <v>2</v>
+      </c>
+      <c r="E32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D33">
+        <v>2</v>
+      </c>
+      <c r="E33">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D34">
+        <v>2</v>
+      </c>
+      <c r="E34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D35">
+        <v>2</v>
+      </c>
+      <c r="E35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D36">
+        <v>2</v>
+      </c>
+      <c r="E36">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D37">
+        <v>2</v>
+      </c>
+      <c r="E37">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D38">
+        <v>2</v>
+      </c>
+      <c r="E38">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D39">
+        <v>2</v>
+      </c>
+      <c r="E39">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D40">
+        <v>2</v>
+      </c>
+      <c r="E40">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D41">
+        <v>2</v>
+      </c>
+      <c r="E41">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D42">
+        <v>2</v>
+      </c>
+      <c r="E42">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D43">
+        <v>2</v>
+      </c>
+      <c r="E43">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D44">
+        <v>2</v>
+      </c>
+      <c r="E44">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D45">
+        <v>2</v>
+      </c>
+      <c r="E45">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D46">
+        <v>2</v>
+      </c>
+      <c r="E46">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D47">
+        <v>2</v>
+      </c>
+      <c r="E47">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D48">
+        <v>2</v>
+      </c>
+      <c r="E48">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D49">
+        <v>2</v>
+      </c>
+      <c r="E49">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D50">
+        <v>2</v>
+      </c>
+      <c r="E50">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D51">
+        <v>2</v>
+      </c>
+      <c r="E51">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D52">
+        <v>2</v>
+      </c>
+      <c r="E52">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D53">
+        <v>2</v>
+      </c>
+      <c r="E53">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D54">
+        <v>2</v>
+      </c>
+      <c r="E54">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D55">
+        <v>2</v>
+      </c>
+      <c r="E55">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D56">
+        <v>2</v>
+      </c>
+      <c r="E56">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D57">
+        <v>2</v>
+      </c>
+      <c r="E57">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D58">
+        <v>2</v>
+      </c>
+      <c r="E58">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D59">
+        <v>2</v>
+      </c>
+      <c r="E59">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D60">
+        <v>2</v>
+      </c>
+      <c r="E60">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D61">
+        <v>2</v>
+      </c>
+      <c r="E61">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C3"/>
@@ -1155,10 +2298,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView topLeftCell="B11" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView topLeftCell="A33" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
+      <selection sqref="A1:E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1358,7 +2501,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="1" t="s">
         <v>60</v>
       </c>
       <c r="B12" t="s">
@@ -1409,7 +2552,7 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="1" t="s">
         <v>64</v>
       </c>
       <c r="B15" t="s">
@@ -1426,7 +2569,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B16" t="s">
@@ -1443,7 +2586,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="1" t="s">
         <v>66</v>
       </c>
       <c r="B17" t="s">
@@ -1626,6 +2769,278 @@
         <v>10</v>
       </c>
       <c r="E27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>181</v>
+      </c>
+      <c r="B28" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28" t="s">
+        <v>61</v>
+      </c>
+      <c r="D28" t="s">
+        <v>34</v>
+      </c>
+      <c r="E28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>182</v>
+      </c>
+      <c r="B29" t="s">
+        <v>31</v>
+      </c>
+      <c r="C29" t="s">
+        <v>35</v>
+      </c>
+      <c r="D29" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>183</v>
+      </c>
+      <c r="B30" t="s">
+        <v>31</v>
+      </c>
+      <c r="C30" t="s">
+        <v>35</v>
+      </c>
+      <c r="D30" t="s">
+        <v>10</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>184</v>
+      </c>
+      <c r="B31" t="s">
+        <v>31</v>
+      </c>
+      <c r="C31" t="s">
+        <v>35</v>
+      </c>
+      <c r="D31" t="s">
+        <v>10</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>185</v>
+      </c>
+      <c r="B32" t="s">
+        <v>31</v>
+      </c>
+      <c r="C32" t="s">
+        <v>35</v>
+      </c>
+      <c r="D32" t="s">
+        <v>10</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>186</v>
+      </c>
+      <c r="B33" t="s">
+        <v>31</v>
+      </c>
+      <c r="C33" t="s">
+        <v>35</v>
+      </c>
+      <c r="D33" t="s">
+        <v>10</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>187</v>
+      </c>
+      <c r="B34" t="s">
+        <v>31</v>
+      </c>
+      <c r="C34" t="s">
+        <v>35</v>
+      </c>
+      <c r="D34" t="s">
+        <v>10</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>188</v>
+      </c>
+      <c r="B35" t="s">
+        <v>31</v>
+      </c>
+      <c r="C35" t="s">
+        <v>35</v>
+      </c>
+      <c r="D35" t="s">
+        <v>10</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>189</v>
+      </c>
+      <c r="B36" t="s">
+        <v>31</v>
+      </c>
+      <c r="C36" t="s">
+        <v>35</v>
+      </c>
+      <c r="D36" t="s">
+        <v>10</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>190</v>
+      </c>
+      <c r="B37" t="s">
+        <v>31</v>
+      </c>
+      <c r="C37" t="s">
+        <v>35</v>
+      </c>
+      <c r="D37" t="s">
+        <v>10</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>191</v>
+      </c>
+      <c r="B38" t="s">
+        <v>142</v>
+      </c>
+      <c r="C38" t="s">
+        <v>35</v>
+      </c>
+      <c r="D38" t="s">
+        <v>10</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>192</v>
+      </c>
+      <c r="B39" t="s">
+        <v>142</v>
+      </c>
+      <c r="C39" t="s">
+        <v>35</v>
+      </c>
+      <c r="D39" t="s">
+        <v>10</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>193</v>
+      </c>
+      <c r="B40" t="s">
+        <v>31</v>
+      </c>
+      <c r="C40" t="s">
+        <v>35</v>
+      </c>
+      <c r="D40" t="s">
+        <v>10</v>
+      </c>
+      <c r="E40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>194</v>
+      </c>
+      <c r="B41" t="s">
+        <v>195</v>
+      </c>
+      <c r="C41" t="s">
+        <v>35</v>
+      </c>
+      <c r="D41" t="s">
+        <v>10</v>
+      </c>
+      <c r="E41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>196</v>
+      </c>
+      <c r="B42" t="s">
+        <v>31</v>
+      </c>
+      <c r="C42" t="s">
+        <v>35</v>
+      </c>
+      <c r="D42" t="s">
+        <v>10</v>
+      </c>
+      <c r="E42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>197</v>
+      </c>
+      <c r="B43" t="s">
+        <v>31</v>
+      </c>
+      <c r="C43" t="s">
+        <v>35</v>
+      </c>
+      <c r="D43" t="s">
+        <v>10</v>
+      </c>
+      <c r="E43">
         <v>1</v>
       </c>
     </row>
@@ -1641,10 +3056,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView zoomScale="141" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection sqref="A1:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1792,6 +3207,20 @@
       </c>
       <c r="D10" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>178</v>
+      </c>
+      <c r="B11" t="s">
+        <v>179</v>
+      </c>
+      <c r="C11" t="s">
+        <v>180</v>
+      </c>
+      <c r="D11" t="s">
+        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -1830,19 +3259,19 @@
       <c r="B1" t="s">
         <v>90</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>143</v>
       </c>
     </row>
@@ -2140,13 +3569,13 @@
       <c r="B1" t="s">
         <v>168</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>171</v>
       </c>
     </row>
@@ -2351,8 +3780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F50DD301-9CCE-6744-864C-185ECBAFA9CA}">
   <dimension ref="A1:G122"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView zoomScale="99" workbookViewId="0">
+      <selection sqref="A1:G122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2391,13 +3820,13 @@
       <c r="A2">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="D2" s="4" t="s">
+      <c r="C2" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>156</v>
       </c>
       <c r="E2">
@@ -2414,13 +3843,13 @@
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="D3" s="4" t="s">
+      <c r="C3" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>156</v>
       </c>
       <c r="E3">
@@ -2437,13 +3866,13 @@
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="D4" s="4" t="s">
+      <c r="C4" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>156</v>
       </c>
       <c r="E4">
@@ -2460,13 +3889,13 @@
       <c r="A5">
         <v>3</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="D5" s="4" t="s">
+      <c r="C5" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>156</v>
       </c>
       <c r="E5">
@@ -2483,13 +3912,13 @@
       <c r="A6">
         <v>4</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="D6" s="4" t="s">
+      <c r="C6" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>156</v>
       </c>
       <c r="E6">
@@ -2506,13 +3935,13 @@
       <c r="A7">
         <v>5</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="D7" s="4" t="s">
+      <c r="C7" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>156</v>
       </c>
       <c r="E7">
@@ -2529,13 +3958,13 @@
       <c r="A8">
         <v>6</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="D8" s="4" t="s">
+      <c r="C8" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>156</v>
       </c>
       <c r="E8">
@@ -2552,13 +3981,13 @@
       <c r="A9">
         <v>7</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="D9" s="4" t="s">
+      <c r="C9" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>156</v>
       </c>
       <c r="E9">
@@ -2575,13 +4004,13 @@
       <c r="A10">
         <v>8</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="D10" s="4" t="s">
+      <c r="C10" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>156</v>
       </c>
       <c r="E10">
@@ -2598,13 +4027,13 @@
       <c r="A11">
         <v>9</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="D11" s="4" t="s">
+      <c r="C11" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>156</v>
       </c>
       <c r="E11">
@@ -2621,13 +4050,13 @@
       <c r="A12">
         <v>10</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="D12" s="4" t="s">
+      <c r="C12" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>156</v>
       </c>
       <c r="E12">
@@ -2644,13 +4073,13 @@
       <c r="A13">
         <v>11</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="D13" s="4" t="s">
+      <c r="C13" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>156</v>
       </c>
       <c r="E13">
@@ -2667,13 +4096,13 @@
       <c r="A14">
         <v>12</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="D14" s="4" t="s">
+      <c r="C14" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>156</v>
       </c>
       <c r="E14">
@@ -2690,13 +4119,13 @@
       <c r="A15">
         <v>13</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="C15" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="D15" s="4" t="s">
+      <c r="C15" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>156</v>
       </c>
       <c r="E15">
@@ -2713,13 +4142,13 @@
       <c r="A16">
         <v>14</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="D16" s="4" t="s">
+      <c r="C16" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>156</v>
       </c>
       <c r="E16">
@@ -2736,13 +4165,13 @@
       <c r="A17">
         <v>15</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="D17" s="4" t="s">
+      <c r="C17" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>156</v>
       </c>
       <c r="E17">
@@ -2759,13 +4188,13 @@
       <c r="A18">
         <v>16</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="D18" s="4" t="s">
+      <c r="C18" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D18" s="3" t="s">
         <v>156</v>
       </c>
       <c r="E18">
@@ -2782,13 +4211,13 @@
       <c r="A19">
         <v>17</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="D19" s="4" t="s">
+      <c r="C19" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D19" s="3" t="s">
         <v>156</v>
       </c>
       <c r="E19">
@@ -2805,13 +4234,13 @@
       <c r="A20">
         <v>18</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="D20" s="4" t="s">
+      <c r="C20" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D20" s="3" t="s">
         <v>156</v>
       </c>
       <c r="E20">
@@ -2828,13 +4257,13 @@
       <c r="A21">
         <v>19</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="C21" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="D21" s="4" t="s">
+      <c r="C21" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D21" s="3" t="s">
         <v>156</v>
       </c>
       <c r="E21">
@@ -2851,13 +4280,13 @@
       <c r="A22">
         <v>20</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="C22" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="D22" s="4" t="s">
+      <c r="C22" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D22" s="3" t="s">
         <v>156</v>
       </c>
       <c r="E22">
@@ -2874,13 +4303,13 @@
       <c r="A23">
         <v>21</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="C23" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="D23" s="4" t="s">
+      <c r="C23" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D23" s="3" t="s">
         <v>156</v>
       </c>
       <c r="E23">
@@ -2897,13 +4326,13 @@
       <c r="A24">
         <v>22</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="C24" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="D24" s="4" t="s">
+      <c r="C24" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D24" s="3" t="s">
         <v>156</v>
       </c>
       <c r="E24">
@@ -2920,13 +4349,13 @@
       <c r="A25">
         <v>23</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="C25" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="D25" s="4" t="s">
+      <c r="C25" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D25" s="3" t="s">
         <v>156</v>
       </c>
       <c r="E25">
@@ -2943,13 +4372,13 @@
       <c r="A26">
         <v>24</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="C26" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="D26" s="4" t="s">
+      <c r="C26" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D26" s="3" t="s">
         <v>156</v>
       </c>
       <c r="E26">
@@ -2966,13 +4395,13 @@
       <c r="A27">
         <v>25</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="C27" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="D27" s="4" t="s">
+      <c r="C27" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D27" s="3" t="s">
         <v>156</v>
       </c>
       <c r="E27">
@@ -2989,13 +4418,13 @@
       <c r="A28">
         <v>26</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="C28" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="D28" s="4" t="s">
+      <c r="C28" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D28" s="3" t="s">
         <v>156</v>
       </c>
       <c r="E28">
@@ -3012,13 +4441,13 @@
       <c r="A29">
         <v>27</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="C29" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="D29" s="4" t="s">
+      <c r="C29" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D29" s="3" t="s">
         <v>156</v>
       </c>
       <c r="E29">
@@ -3035,13 +4464,13 @@
       <c r="A30">
         <v>28</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="C30" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="D30" s="4" t="s">
+      <c r="C30" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D30" s="3" t="s">
         <v>156</v>
       </c>
       <c r="E30">
@@ -3058,13 +4487,13 @@
       <c r="A31">
         <v>29</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="C31" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="D31" s="4" t="s">
+      <c r="C31" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D31" s="3" t="s">
         <v>156</v>
       </c>
       <c r="E31">
@@ -3081,13 +4510,13 @@
       <c r="A32">
         <v>30</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="C32" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="D32" s="4" t="s">
+      <c r="C32" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D32" s="3" t="s">
         <v>156</v>
       </c>
       <c r="E32">
@@ -3104,13 +4533,13 @@
       <c r="A33">
         <v>31</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B33" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="C33" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="D33" s="4" t="s">
+      <c r="C33" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D33" s="3" t="s">
         <v>156</v>
       </c>
       <c r="E33">
@@ -3127,13 +4556,13 @@
       <c r="A34">
         <v>32</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B34" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="C34" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="D34" s="4" t="s">
+      <c r="C34" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D34" s="3" t="s">
         <v>156</v>
       </c>
       <c r="E34">
@@ -3150,13 +4579,13 @@
       <c r="A35">
         <v>33</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B35" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="C35" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="D35" s="4" t="s">
+      <c r="C35" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D35" s="3" t="s">
         <v>156</v>
       </c>
       <c r="E35">
@@ -3173,13 +4602,13 @@
       <c r="A36">
         <v>34</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B36" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="C36" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="D36" s="4" t="s">
+      <c r="C36" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D36" s="3" t="s">
         <v>156</v>
       </c>
       <c r="E36">
@@ -3196,13 +4625,13 @@
       <c r="A37">
         <v>35</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B37" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="C37" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="D37" s="4" t="s">
+      <c r="C37" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D37" s="3" t="s">
         <v>156</v>
       </c>
       <c r="E37">
@@ -3219,13 +4648,13 @@
       <c r="A38">
         <v>36</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B38" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="C38" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="D38" s="4" t="s">
+      <c r="C38" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D38" s="3" t="s">
         <v>156</v>
       </c>
       <c r="E38">
@@ -3242,13 +4671,13 @@
       <c r="A39">
         <v>37</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="B39" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="C39" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="D39" s="4" t="s">
+      <c r="C39" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D39" s="3" t="s">
         <v>156</v>
       </c>
       <c r="E39">
@@ -3265,13 +4694,13 @@
       <c r="A40">
         <v>38</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B40" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="C40" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="D40" s="4" t="s">
+      <c r="C40" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D40" s="3" t="s">
         <v>156</v>
       </c>
       <c r="E40">
@@ -3288,13 +4717,13 @@
       <c r="A41">
         <v>39</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="B41" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="C41" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="D41" s="4" t="s">
+      <c r="C41" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D41" s="3" t="s">
         <v>156</v>
       </c>
       <c r="E41">
@@ -3311,13 +4740,13 @@
       <c r="A42">
         <v>40</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="B42" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="C42" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="D42" s="4" t="s">
+      <c r="C42" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D42" s="3" t="s">
         <v>156</v>
       </c>
       <c r="E42">
@@ -3334,13 +4763,13 @@
       <c r="A43">
         <v>41</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="B43" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="C43" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="D43" s="4" t="s">
+      <c r="C43" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D43" s="3" t="s">
         <v>156</v>
       </c>
       <c r="E43">
@@ -3357,13 +4786,13 @@
       <c r="A44">
         <v>42</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="B44" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="C44" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="D44" s="4" t="s">
+      <c r="C44" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D44" s="3" t="s">
         <v>156</v>
       </c>
       <c r="E44">
@@ -3380,13 +4809,13 @@
       <c r="A45">
         <v>43</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="B45" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="C45" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="D45" s="4" t="s">
+      <c r="C45" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D45" s="3" t="s">
         <v>156</v>
       </c>
       <c r="E45">
@@ -3403,13 +4832,13 @@
       <c r="A46">
         <v>44</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="B46" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="C46" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="D46" s="4" t="s">
+      <c r="C46" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D46" s="3" t="s">
         <v>156</v>
       </c>
       <c r="E46">
@@ -3426,13 +4855,13 @@
       <c r="A47">
         <v>45</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B47" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="C47" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="D47" s="4" t="s">
+      <c r="C47" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D47" s="3" t="s">
         <v>156</v>
       </c>
       <c r="E47">
@@ -3449,13 +4878,13 @@
       <c r="A48">
         <v>46</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="B48" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="C48" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="D48" s="4" t="s">
+      <c r="C48" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D48" s="3" t="s">
         <v>156</v>
       </c>
       <c r="E48">
@@ -3472,13 +4901,13 @@
       <c r="A49">
         <v>47</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="B49" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="C49" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="D49" s="4" t="s">
+      <c r="C49" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D49" s="3" t="s">
         <v>156</v>
       </c>
       <c r="E49">
@@ -3495,13 +4924,13 @@
       <c r="A50">
         <v>48</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="B50" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="C50" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="D50" s="4" t="s">
+      <c r="C50" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D50" s="3" t="s">
         <v>156</v>
       </c>
       <c r="E50">
@@ -3518,13 +4947,13 @@
       <c r="A51">
         <v>49</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="B51" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="C51" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="D51" s="4" t="s">
+      <c r="C51" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D51" s="3" t="s">
         <v>156</v>
       </c>
       <c r="E51">
@@ -3541,13 +4970,13 @@
       <c r="A52">
         <v>50</v>
       </c>
-      <c r="B52" s="4" t="s">
+      <c r="B52" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="C52" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="D52" s="4" t="s">
+      <c r="C52" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D52" s="3" t="s">
         <v>156</v>
       </c>
       <c r="E52">
@@ -3564,13 +4993,13 @@
       <c r="A53">
         <v>51</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="B53" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="C53" s="4" t="s">
+      <c r="C53" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="D53" s="4" t="s">
+      <c r="D53" s="3" t="s">
         <v>159</v>
       </c>
       <c r="E53">
@@ -3587,13 +5016,13 @@
       <c r="A54">
         <v>52</v>
       </c>
-      <c r="B54" s="4" t="s">
+      <c r="B54" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="C54" s="4" t="s">
+      <c r="C54" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="D54" s="4" t="s">
+      <c r="D54" s="3" t="s">
         <v>159</v>
       </c>
       <c r="E54">
@@ -3610,13 +5039,13 @@
       <c r="A55">
         <v>53</v>
       </c>
-      <c r="B55" s="4" t="s">
+      <c r="B55" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="C55" s="4" t="s">
+      <c r="C55" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="D55" s="4" t="s">
+      <c r="D55" s="3" t="s">
         <v>159</v>
       </c>
       <c r="E55">
@@ -3633,13 +5062,13 @@
       <c r="A56">
         <v>54</v>
       </c>
-      <c r="B56" s="4" t="s">
+      <c r="B56" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="C56" s="4" t="s">
+      <c r="C56" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="D56" s="4" t="s">
+      <c r="D56" s="3" t="s">
         <v>159</v>
       </c>
       <c r="E56">
@@ -3656,13 +5085,13 @@
       <c r="A57">
         <v>55</v>
       </c>
-      <c r="B57" s="4" t="s">
+      <c r="B57" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="C57" s="4" t="s">
+      <c r="C57" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="D57" s="4" t="s">
+      <c r="D57" s="3" t="s">
         <v>159</v>
       </c>
       <c r="E57">
@@ -3679,13 +5108,13 @@
       <c r="A58">
         <v>56</v>
       </c>
-      <c r="B58" s="4" t="s">
+      <c r="B58" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="C58" s="4" t="s">
+      <c r="C58" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="D58" s="4" t="s">
+      <c r="D58" s="3" t="s">
         <v>159</v>
       </c>
       <c r="E58">
@@ -3702,13 +5131,13 @@
       <c r="A59">
         <v>57</v>
       </c>
-      <c r="B59" s="4" t="s">
+      <c r="B59" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="C59" s="4" t="s">
+      <c r="C59" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="D59" s="4" t="s">
+      <c r="D59" s="3" t="s">
         <v>159</v>
       </c>
       <c r="E59">
@@ -3725,13 +5154,13 @@
       <c r="A60">
         <v>58</v>
       </c>
-      <c r="B60" s="4" t="s">
+      <c r="B60" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="C60" s="4" t="s">
+      <c r="C60" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="D60" s="4" t="s">
+      <c r="D60" s="3" t="s">
         <v>159</v>
       </c>
       <c r="E60">
@@ -3748,13 +5177,13 @@
       <c r="A61">
         <v>59</v>
       </c>
-      <c r="B61" s="4" t="s">
+      <c r="B61" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="C61" s="4" t="s">
+      <c r="C61" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="D61" s="4" t="s">
+      <c r="D61" s="3" t="s">
         <v>159</v>
       </c>
       <c r="E61">
@@ -3771,13 +5200,13 @@
       <c r="A62">
         <v>60</v>
       </c>
-      <c r="B62" s="4" t="s">
+      <c r="B62" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="C62" s="4" t="s">
+      <c r="C62" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="D62" s="4" t="s">
+      <c r="D62" s="3" t="s">
         <v>159</v>
       </c>
       <c r="E62">
@@ -3794,13 +5223,13 @@
       <c r="A63">
         <v>61</v>
       </c>
-      <c r="B63" s="4" t="s">
+      <c r="B63" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="C63" s="4" t="s">
+      <c r="C63" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="D63" s="4" t="s">
+      <c r="D63" s="3" t="s">
         <v>159</v>
       </c>
       <c r="E63">
@@ -3817,13 +5246,13 @@
       <c r="A64">
         <v>62</v>
       </c>
-      <c r="B64" s="4" t="s">
+      <c r="B64" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="C64" s="4" t="s">
+      <c r="C64" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="D64" s="4" t="s">
+      <c r="D64" s="3" t="s">
         <v>159</v>
       </c>
       <c r="E64">
@@ -3840,13 +5269,13 @@
       <c r="A65">
         <v>63</v>
       </c>
-      <c r="B65" s="4" t="s">
+      <c r="B65" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="C65" s="4" t="s">
+      <c r="C65" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="D65" s="4" t="s">
+      <c r="D65" s="3" t="s">
         <v>159</v>
       </c>
       <c r="E65">
@@ -3863,13 +5292,13 @@
       <c r="A66">
         <v>64</v>
       </c>
-      <c r="B66" s="4" t="s">
+      <c r="B66" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="C66" s="4" t="s">
+      <c r="C66" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="D66" s="4" t="s">
+      <c r="D66" s="3" t="s">
         <v>159</v>
       </c>
       <c r="E66">
@@ -3886,13 +5315,13 @@
       <c r="A67">
         <v>65</v>
       </c>
-      <c r="B67" s="4" t="s">
+      <c r="B67" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="C67" s="4" t="s">
+      <c r="C67" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="D67" s="4" t="s">
+      <c r="D67" s="3" t="s">
         <v>159</v>
       </c>
       <c r="E67">
@@ -3909,13 +5338,13 @@
       <c r="A68">
         <v>66</v>
       </c>
-      <c r="B68" s="4" t="s">
+      <c r="B68" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="C68" s="4" t="s">
+      <c r="C68" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="D68" s="4" t="s">
+      <c r="D68" s="3" t="s">
         <v>159</v>
       </c>
       <c r="E68">
@@ -3932,13 +5361,13 @@
       <c r="A69">
         <v>67</v>
       </c>
-      <c r="B69" s="4" t="s">
+      <c r="B69" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="C69" s="4" t="s">
+      <c r="C69" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="D69" s="4" t="s">
+      <c r="D69" s="3" t="s">
         <v>159</v>
       </c>
       <c r="E69">
@@ -3955,13 +5384,13 @@
       <c r="A70">
         <v>68</v>
       </c>
-      <c r="B70" s="4" t="s">
+      <c r="B70" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="C70" s="4" t="s">
+      <c r="C70" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="D70" s="4" t="s">
+      <c r="D70" s="3" t="s">
         <v>159</v>
       </c>
       <c r="E70">
@@ -3978,13 +5407,13 @@
       <c r="A71">
         <v>69</v>
       </c>
-      <c r="B71" s="4" t="s">
+      <c r="B71" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="C71" s="4" t="s">
+      <c r="C71" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="D71" s="4" t="s">
+      <c r="D71" s="3" t="s">
         <v>159</v>
       </c>
       <c r="E71">
@@ -4001,13 +5430,13 @@
       <c r="A72">
         <v>70</v>
       </c>
-      <c r="B72" s="4" t="s">
+      <c r="B72" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="C72" s="4" t="s">
+      <c r="C72" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="D72" s="4" t="s">
+      <c r="D72" s="3" t="s">
         <v>159</v>
       </c>
       <c r="E72">
@@ -4024,13 +5453,13 @@
       <c r="A73">
         <v>71</v>
       </c>
-      <c r="B73" s="4" t="s">
+      <c r="B73" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="C73" s="4" t="s">
+      <c r="C73" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="D73" s="4" t="s">
+      <c r="D73" s="3" t="s">
         <v>159</v>
       </c>
       <c r="E73">
@@ -4047,13 +5476,13 @@
       <c r="A74">
         <v>72</v>
       </c>
-      <c r="B74" s="4" t="s">
+      <c r="B74" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="C74" s="4" t="s">
+      <c r="C74" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="D74" s="4" t="s">
+      <c r="D74" s="3" t="s">
         <v>159</v>
       </c>
       <c r="E74">
@@ -4070,13 +5499,13 @@
       <c r="A75">
         <v>73</v>
       </c>
-      <c r="B75" s="4" t="s">
+      <c r="B75" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="C75" s="4" t="s">
+      <c r="C75" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="D75" s="4" t="s">
+      <c r="D75" s="3" t="s">
         <v>159</v>
       </c>
       <c r="E75">
@@ -4093,13 +5522,13 @@
       <c r="A76">
         <v>74</v>
       </c>
-      <c r="B76" s="4" t="s">
+      <c r="B76" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="C76" s="4" t="s">
+      <c r="C76" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="D76" s="4" t="s">
+      <c r="D76" s="3" t="s">
         <v>159</v>
       </c>
       <c r="E76">
@@ -4116,13 +5545,13 @@
       <c r="A77">
         <v>75</v>
       </c>
-      <c r="B77" s="4" t="s">
+      <c r="B77" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="C77" s="4" t="s">
+      <c r="C77" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="D77" s="4" t="s">
+      <c r="D77" s="3" t="s">
         <v>159</v>
       </c>
       <c r="E77">
@@ -4139,13 +5568,13 @@
       <c r="A78">
         <v>76</v>
       </c>
-      <c r="B78" s="4" t="s">
+      <c r="B78" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="C78" s="4" t="s">
+      <c r="C78" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="D78" s="4" t="s">
+      <c r="D78" s="3" t="s">
         <v>159</v>
       </c>
       <c r="E78">
@@ -4162,13 +5591,13 @@
       <c r="A79">
         <v>77</v>
       </c>
-      <c r="B79" s="4" t="s">
+      <c r="B79" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="C79" s="4" t="s">
+      <c r="C79" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="D79" s="4" t="s">
+      <c r="D79" s="3" t="s">
         <v>159</v>
       </c>
       <c r="E79">
@@ -4185,13 +5614,13 @@
       <c r="A80">
         <v>78</v>
       </c>
-      <c r="B80" s="4" t="s">
+      <c r="B80" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="C80" s="4" t="s">
+      <c r="C80" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="D80" s="4" t="s">
+      <c r="D80" s="3" t="s">
         <v>159</v>
       </c>
       <c r="E80">
@@ -4208,13 +5637,13 @@
       <c r="A81">
         <v>79</v>
       </c>
-      <c r="B81" s="4" t="s">
+      <c r="B81" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="C81" s="4" t="s">
+      <c r="C81" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="D81" s="4" t="s">
+      <c r="D81" s="3" t="s">
         <v>159</v>
       </c>
       <c r="E81">
@@ -4231,13 +5660,13 @@
       <c r="A82">
         <v>80</v>
       </c>
-      <c r="B82" s="4" t="s">
+      <c r="B82" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="C82" s="4" t="s">
+      <c r="C82" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="D82" s="4" t="s">
+      <c r="D82" s="3" t="s">
         <v>159</v>
       </c>
       <c r="E82">
@@ -4254,13 +5683,13 @@
       <c r="A83">
         <v>81</v>
       </c>
-      <c r="B83" s="4" t="s">
+      <c r="B83" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="C83" s="4" t="s">
+      <c r="C83" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="D83" s="4" t="s">
+      <c r="D83" s="3" t="s">
         <v>159</v>
       </c>
       <c r="E83">
@@ -4277,13 +5706,13 @@
       <c r="A84">
         <v>82</v>
       </c>
-      <c r="B84" s="4" t="s">
+      <c r="B84" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="C84" s="4" t="s">
+      <c r="C84" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="D84" s="4" t="s">
+      <c r="D84" s="3" t="s">
         <v>159</v>
       </c>
       <c r="E84">
@@ -4300,13 +5729,13 @@
       <c r="A85">
         <v>83</v>
       </c>
-      <c r="B85" s="4" t="s">
+      <c r="B85" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="C85" s="4" t="s">
+      <c r="C85" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="D85" s="4" t="s">
+      <c r="D85" s="3" t="s">
         <v>159</v>
       </c>
       <c r="E85">
@@ -4323,13 +5752,13 @@
       <c r="A86">
         <v>84</v>
       </c>
-      <c r="B86" s="4" t="s">
+      <c r="B86" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="C86" s="4" t="s">
+      <c r="C86" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="D86" s="4" t="s">
+      <c r="D86" s="3" t="s">
         <v>159</v>
       </c>
       <c r="E86">
@@ -4346,13 +5775,13 @@
       <c r="A87">
         <v>85</v>
       </c>
-      <c r="B87" s="4" t="s">
+      <c r="B87" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="C87" s="4" t="s">
+      <c r="C87" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="D87" s="4" t="s">
+      <c r="D87" s="3" t="s">
         <v>159</v>
       </c>
       <c r="E87">
@@ -4369,13 +5798,13 @@
       <c r="A88">
         <v>86</v>
       </c>
-      <c r="B88" s="4" t="s">
+      <c r="B88" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="C88" s="4" t="s">
+      <c r="C88" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="D88" s="4" t="s">
+      <c r="D88" s="3" t="s">
         <v>159</v>
       </c>
       <c r="E88">
@@ -4392,13 +5821,13 @@
       <c r="A89">
         <v>87</v>
       </c>
-      <c r="B89" s="4" t="s">
+      <c r="B89" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="C89" s="4" t="s">
+      <c r="C89" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="D89" s="4" t="s">
+      <c r="D89" s="3" t="s">
         <v>159</v>
       </c>
       <c r="E89">
@@ -4415,13 +5844,13 @@
       <c r="A90">
         <v>88</v>
       </c>
-      <c r="B90" s="4" t="s">
+      <c r="B90" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="C90" s="4" t="s">
+      <c r="C90" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="D90" s="4" t="s">
+      <c r="D90" s="3" t="s">
         <v>159</v>
       </c>
       <c r="E90">
@@ -4438,13 +5867,13 @@
       <c r="A91">
         <v>89</v>
       </c>
-      <c r="B91" s="4" t="s">
+      <c r="B91" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="C91" s="4" t="s">
+      <c r="C91" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="D91" s="4" t="s">
+      <c r="D91" s="3" t="s">
         <v>159</v>
       </c>
       <c r="E91">
@@ -4461,13 +5890,13 @@
       <c r="A92">
         <v>90</v>
       </c>
-      <c r="B92" s="4" t="s">
+      <c r="B92" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="C92" s="4" t="s">
+      <c r="C92" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="D92" s="4" t="s">
+      <c r="D92" s="3" t="s">
         <v>159</v>
       </c>
       <c r="E92">
@@ -4484,13 +5913,13 @@
       <c r="A93">
         <v>91</v>
       </c>
-      <c r="B93" s="4" t="s">
+      <c r="B93" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="C93" s="4" t="s">
+      <c r="C93" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="D93" s="4" t="s">
+      <c r="D93" s="3" t="s">
         <v>159</v>
       </c>
       <c r="E93">
@@ -4507,13 +5936,13 @@
       <c r="A94">
         <v>92</v>
       </c>
-      <c r="B94" s="4" t="s">
+      <c r="B94" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="C94" s="4" t="s">
+      <c r="C94" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="D94" s="4" t="s">
+      <c r="D94" s="3" t="s">
         <v>159</v>
       </c>
       <c r="E94">
@@ -4530,13 +5959,13 @@
       <c r="A95">
         <v>93</v>
       </c>
-      <c r="B95" s="4" t="s">
+      <c r="B95" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="C95" s="4" t="s">
+      <c r="C95" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="D95" s="4" t="s">
+      <c r="D95" s="3" t="s">
         <v>159</v>
       </c>
       <c r="E95">
@@ -4553,13 +5982,13 @@
       <c r="A96">
         <v>94</v>
       </c>
-      <c r="B96" s="4" t="s">
+      <c r="B96" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="C96" s="4" t="s">
+      <c r="C96" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="D96" s="4" t="s">
+      <c r="D96" s="3" t="s">
         <v>159</v>
       </c>
       <c r="E96">
@@ -4576,13 +6005,13 @@
       <c r="A97">
         <v>95</v>
       </c>
-      <c r="B97" s="4" t="s">
+      <c r="B97" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="C97" s="4" t="s">
+      <c r="C97" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="D97" s="4" t="s">
+      <c r="D97" s="3" t="s">
         <v>159</v>
       </c>
       <c r="E97">
@@ -4599,13 +6028,13 @@
       <c r="A98">
         <v>96</v>
       </c>
-      <c r="B98" s="4" t="s">
+      <c r="B98" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="C98" s="4" t="s">
+      <c r="C98" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="D98" s="4" t="s">
+      <c r="D98" s="3" t="s">
         <v>159</v>
       </c>
       <c r="E98">
@@ -4622,13 +6051,13 @@
       <c r="A99">
         <v>97</v>
       </c>
-      <c r="B99" s="4" t="s">
+      <c r="B99" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="C99" s="4" t="s">
+      <c r="C99" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="D99" s="4" t="s">
+      <c r="D99" s="3" t="s">
         <v>159</v>
       </c>
       <c r="E99">
@@ -4645,13 +6074,13 @@
       <c r="A100">
         <v>98</v>
       </c>
-      <c r="B100" s="4" t="s">
+      <c r="B100" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="C100" s="4" t="s">
+      <c r="C100" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="D100" s="4" t="s">
+      <c r="D100" s="3" t="s">
         <v>159</v>
       </c>
       <c r="E100">
@@ -4668,13 +6097,13 @@
       <c r="A101">
         <v>99</v>
       </c>
-      <c r="B101" s="4" t="s">
+      <c r="B101" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="C101" s="4" t="s">
+      <c r="C101" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="D101" s="4" t="s">
+      <c r="D101" s="3" t="s">
         <v>159</v>
       </c>
       <c r="E101">
@@ -4691,13 +6120,13 @@
       <c r="A102">
         <v>100</v>
       </c>
-      <c r="B102" s="4" t="s">
+      <c r="B102" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="C102" s="4" t="s">
+      <c r="C102" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="D102" s="4" t="s">
+      <c r="D102" s="3" t="s">
         <v>159</v>
       </c>
       <c r="E102">
@@ -4714,13 +6143,13 @@
       <c r="A103">
         <v>101</v>
       </c>
-      <c r="B103" s="4" t="s">
+      <c r="B103" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="C103" s="4" t="s">
+      <c r="C103" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="D103" s="4" t="s">
+      <c r="D103" s="3" t="s">
         <v>159</v>
       </c>
       <c r="E103">
@@ -4737,13 +6166,13 @@
       <c r="A104">
         <v>102</v>
       </c>
-      <c r="B104" s="4" t="s">
+      <c r="B104" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="C104" s="4" t="s">
+      <c r="C104" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="D104" s="4" t="s">
+      <c r="D104" s="3" t="s">
         <v>159</v>
       </c>
       <c r="E104">
@@ -4760,13 +6189,13 @@
       <c r="A105">
         <v>103</v>
       </c>
-      <c r="B105" s="4" t="s">
+      <c r="B105" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="C105" s="4" t="s">
+      <c r="C105" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="D105" s="4" t="s">
+      <c r="D105" s="3" t="s">
         <v>159</v>
       </c>
       <c r="E105">
@@ -4783,13 +6212,13 @@
       <c r="A106">
         <v>104</v>
       </c>
-      <c r="B106" s="4" t="s">
+      <c r="B106" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="C106" s="4" t="s">
+      <c r="C106" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="D106" s="4" t="s">
+      <c r="D106" s="3" t="s">
         <v>159</v>
       </c>
       <c r="E106">
@@ -4806,13 +6235,13 @@
       <c r="A107">
         <v>105</v>
       </c>
-      <c r="B107" s="4" t="s">
+      <c r="B107" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="C107" s="4" t="s">
+      <c r="C107" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="D107" s="4" t="s">
+      <c r="D107" s="3" t="s">
         <v>159</v>
       </c>
       <c r="E107">
@@ -4829,13 +6258,13 @@
       <c r="A108">
         <v>106</v>
       </c>
-      <c r="B108" s="4" t="s">
+      <c r="B108" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="C108" s="4" t="s">
+      <c r="C108" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="D108" s="4" t="s">
+      <c r="D108" s="3" t="s">
         <v>159</v>
       </c>
       <c r="E108">
@@ -4852,13 +6281,13 @@
       <c r="A109">
         <v>107</v>
       </c>
-      <c r="B109" s="4" t="s">
+      <c r="B109" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="C109" s="4" t="s">
+      <c r="C109" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="D109" s="4" t="s">
+      <c r="D109" s="3" t="s">
         <v>159</v>
       </c>
       <c r="E109">
@@ -4875,13 +6304,13 @@
       <c r="A110">
         <v>108</v>
       </c>
-      <c r="B110" s="4" t="s">
+      <c r="B110" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="C110" s="4" t="s">
+      <c r="C110" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="D110" s="4" t="s">
+      <c r="D110" s="3" t="s">
         <v>159</v>
       </c>
       <c r="E110">
@@ -4898,13 +6327,13 @@
       <c r="A111">
         <v>109</v>
       </c>
-      <c r="B111" s="4" t="s">
+      <c r="B111" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="C111" s="4" t="s">
+      <c r="C111" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="D111" s="4" t="s">
+      <c r="D111" s="3" t="s">
         <v>159</v>
       </c>
       <c r="E111">
@@ -4921,13 +6350,13 @@
       <c r="A112">
         <v>110</v>
       </c>
-      <c r="B112" s="4" t="s">
+      <c r="B112" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="C112" s="4" t="s">
+      <c r="C112" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="D112" s="4" t="s">
+      <c r="D112" s="3" t="s">
         <v>159</v>
       </c>
       <c r="E112">
@@ -4944,13 +6373,13 @@
       <c r="A113">
         <v>111</v>
       </c>
-      <c r="B113" s="4" t="s">
+      <c r="B113" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="C113" s="4" t="s">
+      <c r="C113" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="D113" s="4" t="s">
+      <c r="D113" s="3" t="s">
         <v>159</v>
       </c>
       <c r="E113">
@@ -4967,13 +6396,13 @@
       <c r="A114">
         <v>112</v>
       </c>
-      <c r="B114" s="4" t="s">
+      <c r="B114" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="C114" s="4" t="s">
+      <c r="C114" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="D114" s="4" t="s">
+      <c r="D114" s="3" t="s">
         <v>159</v>
       </c>
       <c r="E114">
@@ -4990,13 +6419,13 @@
       <c r="A115">
         <v>113</v>
       </c>
-      <c r="B115" s="4" t="s">
+      <c r="B115" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="C115" s="4" t="s">
+      <c r="C115" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="D115" s="4" t="s">
+      <c r="D115" s="3" t="s">
         <v>159</v>
       </c>
       <c r="E115">
@@ -5013,13 +6442,13 @@
       <c r="A116">
         <v>114</v>
       </c>
-      <c r="B116" s="4" t="s">
+      <c r="B116" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="C116" s="4" t="s">
+      <c r="C116" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="D116" s="4" t="s">
+      <c r="D116" s="3" t="s">
         <v>159</v>
       </c>
       <c r="E116">
@@ -5036,13 +6465,13 @@
       <c r="A117">
         <v>115</v>
       </c>
-      <c r="B117" s="4" t="s">
+      <c r="B117" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="C117" s="4" t="s">
+      <c r="C117" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="D117" s="4" t="s">
+      <c r="D117" s="3" t="s">
         <v>159</v>
       </c>
       <c r="E117">
@@ -5059,13 +6488,13 @@
       <c r="A118">
         <v>116</v>
       </c>
-      <c r="B118" s="4" t="s">
+      <c r="B118" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="C118" s="4" t="s">
+      <c r="C118" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="D118" s="4" t="s">
+      <c r="D118" s="3" t="s">
         <v>159</v>
       </c>
       <c r="E118">
@@ -5082,13 +6511,13 @@
       <c r="A119">
         <v>117</v>
       </c>
-      <c r="B119" s="4" t="s">
+      <c r="B119" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="C119" s="4" t="s">
+      <c r="C119" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="D119" s="4" t="s">
+      <c r="D119" s="3" t="s">
         <v>159</v>
       </c>
       <c r="E119">
@@ -5105,13 +6534,13 @@
       <c r="A120">
         <v>118</v>
       </c>
-      <c r="B120" s="4" t="s">
+      <c r="B120" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="C120" s="4" t="s">
+      <c r="C120" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="D120" s="4" t="s">
+      <c r="D120" s="3" t="s">
         <v>159</v>
       </c>
       <c r="E120">
@@ -5128,13 +6557,13 @@
       <c r="A121">
         <v>119</v>
       </c>
-      <c r="B121" s="4" t="s">
+      <c r="B121" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="C121" s="4" t="s">
+      <c r="C121" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="D121" s="4" t="s">
+      <c r="D121" s="3" t="s">
         <v>159</v>
       </c>
       <c r="E121">
@@ -5151,13 +6580,13 @@
       <c r="A122">
         <v>120</v>
       </c>
-      <c r="B122" s="4" t="s">
+      <c r="B122" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="C122" s="4" t="s">
+      <c r="C122" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="D122" s="4" t="s">
+      <c r="D122" s="3" t="s">
         <v>159</v>
       </c>
       <c r="E122">

</xml_diff>

<commit_message>
los to 59 instead of 60
</commit_message>
<xml_diff>
--- a/lsh_data_processing/lsh_coding.xlsx
+++ b/lsh_data_processing/lsh_coding.xlsx
@@ -5,12 +5,12 @@
   <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/solviro/Documents/COVID-19/BCS/lsh_data_processing/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rjs/projects/covid/BCS/lsh_data_processing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B7795B1-AC91-7C49-A5ED-3940C38F223A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DCFD666-924E-B14F-8872-A39623D4B1AB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-35380" yWindow="460" windowWidth="25600" windowHeight="14540" firstSheet="3" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="660" yWindow="-20220" windowWidth="25600" windowHeight="14540" firstSheet="3" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="lsh_covid_groups" sheetId="3" r:id="rId1"/>
@@ -24,7 +24,7 @@
     <sheet name="age_groups" sheetId="9" r:id="rId9"/>
     <sheet name="length_of_stay_categories" sheetId="10" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="140001"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="826" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="824" uniqueCount="207">
   <si>
     <t>text_out_category_raw</t>
   </si>
@@ -1182,10 +1182,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85754964-25F9-724F-B597-4C81CCFECB89}">
-  <dimension ref="A1:E61"/>
+  <dimension ref="A1:E60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="E68" sqref="E68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2212,23 +2212,6 @@
         <v>2</v>
       </c>
       <c r="E60">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A61">
-        <v>60</v>
-      </c>
-      <c r="B61" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="D61">
-        <v>2</v>
-      </c>
-      <c r="E61">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added unit categories from isolation data
</commit_message>
<xml_diff>
--- a/lsh_data_processing/lsh_coding.xlsx
+++ b/lsh_data_processing/lsh_coding.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rjs/projects/covid/BCS/lsh_data_processing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC19427A-87A5-D640-AC4D-A96F39B4EA30}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E773281-35C3-E243-869E-C5266CE9599A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6880" yWindow="-16000" windowWidth="25600" windowHeight="14320" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9000" yWindow="-16180" windowWidth="25600" windowHeight="14320" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="lsh_covid_groups" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1102" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1186" uniqueCount="276">
   <si>
     <t>text_out_category_raw</t>
   </si>
@@ -795,6 +795,75 @@
   </si>
   <si>
     <t>inpatient_ward_pediadric</t>
+  </si>
+  <si>
+    <t>Hjartadeild (Hb-14EG)</t>
+  </si>
+  <si>
+    <t>Heila-, tauga- og bæklunarskurðdeild (Fv-B6)</t>
+  </si>
+  <si>
+    <t>Móttökugeðdeild (Hb-33A)</t>
+  </si>
+  <si>
+    <t>Sérhæfð endurhæfingargeðdeild (Kl-10C)</t>
+  </si>
+  <si>
+    <t>Móttaka bráða- og göngudeildar (Fv-G2/G3)</t>
+  </si>
+  <si>
+    <t>Móttaka lyf- og skurðlækninga Fossvogi</t>
+  </si>
+  <si>
+    <t>Bráðageðdeild 32C (Hb-32C)</t>
+  </si>
+  <si>
+    <t>Útskriftardeild aldraðra (Lk-L2)</t>
+  </si>
+  <si>
+    <t>Gigtar-og almenn lyflækningadeild (Fv-B7)</t>
+  </si>
+  <si>
+    <t>HNE-, lýta- og æðaskurðdeild (Fv-A4)</t>
+  </si>
+  <si>
+    <t>Kvenlækningadeild (Hb-21A)</t>
+  </si>
+  <si>
+    <t>Bráðalyflækningadeild (Fv-A2)</t>
+  </si>
+  <si>
+    <t>Göngudeild og bráðamóttaka BH (Hb-20E/D)</t>
+  </si>
+  <si>
+    <t>Taugalækningadeild (Fv-B2)</t>
+  </si>
+  <si>
+    <t>Endurhæfingardeild (Gr-R2)</t>
+  </si>
+  <si>
+    <t>Líknardeild, legudeild (Kv-h10-1h)</t>
+  </si>
+  <si>
+    <t>Dag- og göngudeild blóð- og krabbameinslækninga (H</t>
+  </si>
+  <si>
+    <t>Blóð- og krabbameinslækningadeild (Hb-11EG)</t>
+  </si>
+  <si>
+    <t>Dagdeild skurðlækninga F, legudeild (Fv-A5)</t>
+  </si>
+  <si>
+    <t>Meltingar- og nýrnadeild (Hb-12E)</t>
+  </si>
+  <si>
+    <t>Vökudeild (Hb-23D)</t>
+  </si>
+  <si>
+    <t>inpatient_ward_transfer</t>
+  </si>
+  <si>
+    <t>inpatient_ward_transfer_geriatric</t>
   </si>
 </sst>
 </file>
@@ -6049,7 +6118,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6120,17 +6189,17 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E60"/>
+  <dimension ref="A1:E81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="C62" sqref="C62"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
+      <selection activeCell="C85" sqref="C85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="36.5" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
-    <col min="3" max="3" width="21.1640625" customWidth="1"/>
+    <col min="3" max="3" width="28.6640625" customWidth="1"/>
     <col min="4" max="4" width="29.83203125" customWidth="1"/>
     <col min="5" max="5" width="25.5" customWidth="1"/>
   </cols>
@@ -6602,7 +6671,7 @@
         <v>30</v>
       </c>
       <c r="C28" t="s">
-        <v>61</v>
+        <v>275</v>
       </c>
       <c r="D28" t="s">
         <v>34</v>
@@ -7153,6 +7222,363 @@
       </c>
       <c r="E60">
         <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>253</v>
+      </c>
+      <c r="B61" t="s">
+        <v>30</v>
+      </c>
+      <c r="C61" t="s">
+        <v>34</v>
+      </c>
+      <c r="D61" t="s">
+        <v>34</v>
+      </c>
+      <c r="E61">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>254</v>
+      </c>
+      <c r="B62" t="s">
+        <v>30</v>
+      </c>
+      <c r="C62" t="s">
+        <v>34</v>
+      </c>
+      <c r="D62" t="s">
+        <v>34</v>
+      </c>
+      <c r="E62">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>255</v>
+      </c>
+      <c r="B63" t="s">
+        <v>31</v>
+      </c>
+      <c r="C63" t="s">
+        <v>35</v>
+      </c>
+      <c r="D63" t="s">
+        <v>10</v>
+      </c>
+      <c r="E63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>256</v>
+      </c>
+      <c r="B64" t="s">
+        <v>31</v>
+      </c>
+      <c r="C64" t="s">
+        <v>35</v>
+      </c>
+      <c r="D64" t="s">
+        <v>10</v>
+      </c>
+      <c r="E64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>257</v>
+      </c>
+      <c r="B65" t="s">
+        <v>29</v>
+      </c>
+      <c r="C65" t="s">
+        <v>33</v>
+      </c>
+      <c r="D65" t="s">
+        <v>10</v>
+      </c>
+      <c r="E65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>258</v>
+      </c>
+      <c r="B66" t="s">
+        <v>31</v>
+      </c>
+      <c r="C66" t="s">
+        <v>35</v>
+      </c>
+      <c r="D66" t="s">
+        <v>10</v>
+      </c>
+      <c r="E66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>259</v>
+      </c>
+      <c r="B67" t="s">
+        <v>29</v>
+      </c>
+      <c r="C67" t="s">
+        <v>33</v>
+      </c>
+      <c r="D67" t="s">
+        <v>10</v>
+      </c>
+      <c r="E67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>260</v>
+      </c>
+      <c r="B68" t="s">
+        <v>31</v>
+      </c>
+      <c r="C68" t="s">
+        <v>35</v>
+      </c>
+      <c r="D68" t="s">
+        <v>10</v>
+      </c>
+      <c r="E68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>261</v>
+      </c>
+      <c r="B69" t="s">
+        <v>30</v>
+      </c>
+      <c r="C69" t="s">
+        <v>34</v>
+      </c>
+      <c r="D69" t="s">
+        <v>34</v>
+      </c>
+      <c r="E69">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>262</v>
+      </c>
+      <c r="B70" t="s">
+        <v>30</v>
+      </c>
+      <c r="C70" t="s">
+        <v>34</v>
+      </c>
+      <c r="D70" t="s">
+        <v>34</v>
+      </c>
+      <c r="E70">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>263</v>
+      </c>
+      <c r="B71" t="s">
+        <v>30</v>
+      </c>
+      <c r="C71" t="s">
+        <v>34</v>
+      </c>
+      <c r="D71" t="s">
+        <v>34</v>
+      </c>
+      <c r="E71">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>264</v>
+      </c>
+      <c r="B72" t="s">
+        <v>30</v>
+      </c>
+      <c r="C72" t="s">
+        <v>274</v>
+      </c>
+      <c r="D72" t="s">
+        <v>34</v>
+      </c>
+      <c r="E72">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>265</v>
+      </c>
+      <c r="B73" t="s">
+        <v>29</v>
+      </c>
+      <c r="C73" t="s">
+        <v>33</v>
+      </c>
+      <c r="D73" t="s">
+        <v>10</v>
+      </c>
+      <c r="E73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>266</v>
+      </c>
+      <c r="B74" t="s">
+        <v>30</v>
+      </c>
+      <c r="C74" t="s">
+        <v>34</v>
+      </c>
+      <c r="D74" t="s">
+        <v>34</v>
+      </c>
+      <c r="E74">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>267</v>
+      </c>
+      <c r="B75" t="s">
+        <v>30</v>
+      </c>
+      <c r="C75" t="s">
+        <v>34</v>
+      </c>
+      <c r="D75" t="s">
+        <v>34</v>
+      </c>
+      <c r="E75">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>268</v>
+      </c>
+      <c r="B76" t="s">
+        <v>30</v>
+      </c>
+      <c r="C76" t="s">
+        <v>34</v>
+      </c>
+      <c r="D76" t="s">
+        <v>34</v>
+      </c>
+      <c r="E76">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>269</v>
+      </c>
+      <c r="B77" t="s">
+        <v>142</v>
+      </c>
+      <c r="C77" t="s">
+        <v>35</v>
+      </c>
+      <c r="D77" t="s">
+        <v>10</v>
+      </c>
+      <c r="E77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>270</v>
+      </c>
+      <c r="B78" t="s">
+        <v>30</v>
+      </c>
+      <c r="C78" t="s">
+        <v>34</v>
+      </c>
+      <c r="D78" t="s">
+        <v>34</v>
+      </c>
+      <c r="E78">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>271</v>
+      </c>
+      <c r="B79" t="s">
+        <v>142</v>
+      </c>
+      <c r="C79" t="s">
+        <v>35</v>
+      </c>
+      <c r="D79" t="s">
+        <v>10</v>
+      </c>
+      <c r="E79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>272</v>
+      </c>
+      <c r="B80" t="s">
+        <v>30</v>
+      </c>
+      <c r="C80" t="s">
+        <v>34</v>
+      </c>
+      <c r="D80" t="s">
+        <v>34</v>
+      </c>
+      <c r="E80">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>273</v>
+      </c>
+      <c r="B81" t="s">
+        <v>30</v>
+      </c>
+      <c r="C81" t="s">
+        <v>252</v>
+      </c>
+      <c r="D81" t="s">
+        <v>34</v>
+      </c>
+      <c r="E81">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added clinically diagnosed to covid groups
</commit_message>
<xml_diff>
--- a/lsh_data_processing/lsh_coding.xlsx
+++ b/lsh_data_processing/lsh_coding.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rjs/projects/covid/BCS/lsh_data_processing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E773281-35C3-E243-869E-C5266CE9599A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF1716EC-061F-F344-8DE6-AE5C502CCDC4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9000" yWindow="-16180" windowWidth="25600" windowHeight="14320" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3260" yWindow="-16140" windowWidth="25600" windowHeight="14320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="lsh_covid_groups" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1186" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1186" uniqueCount="278">
   <si>
     <t>text_out_category_raw</t>
   </si>
@@ -864,6 +864,12 @@
   </si>
   <si>
     <t>inpatient_ward_transfer_geriatric</t>
+  </si>
+  <si>
+    <t>clinically_diagnosed</t>
+  </si>
+  <si>
+    <t>Klínískt greindir</t>
   </si>
 </sst>
 </file>
@@ -1316,8 +1322,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1376,10 +1382,10 @@
         <v>43</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>46</v>
+        <v>277</v>
       </c>
       <c r="C5" t="s">
-        <v>45</v>
+        <v>276</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -1387,10 +1393,10 @@
         <v>44</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>46</v>
+        <v>277</v>
       </c>
       <c r="C6" t="s">
-        <v>45</v>
+        <v>276</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -6191,7 +6197,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
+    <sheetView topLeftCell="A3" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
       <selection activeCell="C85" sqref="C85"/>
     </sheetView>
   </sheetViews>

</xml_diff>